<commit_message>
Update font and ASM
</commit_message>
<xml_diff>
--- a/2_translated/font/VWF_Properties.xlsx
+++ b/2_translated/font/VWF_Properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forti\Documents\GitHub\Super-Robot-Wars-Z\2_translated\font\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9A9CC6-C9EF-4F1E-B0C2-FC74C0213E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1934B8BA-6B0E-4006-BAB3-3D57ED7D4E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4CE9F589-6C49-444B-92C3-C90A26708452}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{4CE9F589-6C49-444B-92C3-C90A26708452}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="88">
   <si>
     <t>Ａ</t>
   </si>
@@ -284,9 +284,6 @@
     <t>06</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
@@ -294,6 +291,15 @@
   </si>
   <si>
     <t>Width_00</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>≥</t>
+  </si>
+  <si>
+    <t>02</t>
   </si>
 </sst>
 </file>
@@ -681,21 +687,21 @@
   <dimension ref="A1:M114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K65" sqref="K65"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" customWidth="1"/>
+    <col min="8" max="8" width="14.26953125" customWidth="1"/>
+    <col min="11" max="11" width="5.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
@@ -715,7 +721,7 @@
         <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>74</v>
@@ -727,7 +733,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
         <f t="shared" ref="A2:A65" si="0">DEC2HEX((B2 - 32)*4+HEX2DEC($M$1))</f>
         <v>43B590</v>
@@ -741,10 +747,10 @@
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" t="s">
-        <v>65</v>
+        <v>87</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="G2" t="s">
         <v>57</v>
@@ -755,7 +761,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>43B594</v>
@@ -783,7 +789,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>43B598</v>
@@ -811,7 +817,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>43B59C</v>
@@ -839,7 +845,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>43B5A0</v>
@@ -867,7 +873,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>43B5A4</v>
@@ -895,7 +901,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>43B5A8</v>
@@ -923,7 +929,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>43B5AC</v>
@@ -951,7 +957,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>43B5B0</v>
@@ -979,7 +985,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>43B5B4</v>
@@ -1007,7 +1013,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>43B5B8</v>
@@ -1035,7 +1041,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>43B5BC</v>
@@ -1063,7 +1069,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>43B5C0</v>
@@ -1091,7 +1097,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>43B5C4</v>
@@ -1119,7 +1125,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>43B5C8</v>
@@ -1147,7 +1153,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>43B5CC</v>
@@ -1175,7 +1181,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>43B5D0</v>
@@ -1191,8 +1197,8 @@
       <c r="E18" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F18" t="s">
-        <v>65</v>
+      <c r="F18" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="G18" t="s">
         <v>57</v>
@@ -1203,7 +1209,7 @@
       <c r="L18" s="1"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>43B5D4</v>
@@ -1219,8 +1225,8 @@
       <c r="E19" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F19" t="s">
-        <v>65</v>
+      <c r="F19" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="G19" t="s">
         <v>57</v>
@@ -1231,7 +1237,7 @@
       <c r="L19" s="1"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>43B5D8</v>
@@ -1247,8 +1253,8 @@
       <c r="E20" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F20" t="s">
-        <v>65</v>
+      <c r="F20" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="G20" t="s">
         <v>57</v>
@@ -1259,7 +1265,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>43B5DC</v>
@@ -1275,8 +1281,8 @@
       <c r="E21" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F21" t="s">
-        <v>65</v>
+      <c r="F21" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="G21" t="s">
         <v>57</v>
@@ -1287,7 +1293,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>43B5E0</v>
@@ -1303,8 +1309,8 @@
       <c r="E22" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F22" t="s">
-        <v>65</v>
+      <c r="F22" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="G22" t="s">
         <v>57</v>
@@ -1315,7 +1321,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>43B5E4</v>
@@ -1331,8 +1337,8 @@
       <c r="E23" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F23" t="s">
-        <v>65</v>
+      <c r="F23" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="G23" t="s">
         <v>57</v>
@@ -1343,7 +1349,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>43B5E8</v>
@@ -1359,8 +1365,8 @@
       <c r="E24" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F24" t="s">
-        <v>65</v>
+      <c r="F24" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="G24" t="s">
         <v>57</v>
@@ -1371,7 +1377,7 @@
       <c r="L24" s="1"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>43B5EC</v>
@@ -1387,8 +1393,8 @@
       <c r="E25" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F25" t="s">
-        <v>65</v>
+      <c r="F25" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="G25" t="s">
         <v>57</v>
@@ -1399,7 +1405,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>43B5F0</v>
@@ -1415,8 +1421,8 @@
       <c r="E26" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F26" t="s">
-        <v>65</v>
+      <c r="F26" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="G26" t="s">
         <v>57</v>
@@ -1427,7 +1433,7 @@
       <c r="L26" s="1"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>43B5F4</v>
@@ -1443,8 +1449,8 @@
       <c r="E27" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F27" t="s">
-        <v>65</v>
+      <c r="F27" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="G27" t="s">
         <v>57</v>
@@ -1455,7 +1461,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>43B5F8</v>
@@ -1483,7 +1489,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>43B5FC</v>
@@ -1511,7 +1517,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="2"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>43B600</v>
@@ -1539,7 +1545,7 @@
       <c r="L30" s="1"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>43B604</v>
@@ -1567,7 +1573,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>43B608</v>
@@ -1595,7 +1601,7 @@
       <c r="L32" s="1"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>43B60C</v>
@@ -1623,7 +1629,7 @@
       <c r="L33" s="1"/>
       <c r="M33" s="2"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>43B610</v>
@@ -1651,7 +1657,7 @@
       <c r="L34" s="1"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>43B614</v>
@@ -1670,10 +1676,10 @@
         <v>65</v>
       </c>
       <c r="F35" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>67</v>
@@ -1683,7 +1689,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>43B618</v>
@@ -1692,7 +1698,7 @@
         <v>66</v>
       </c>
       <c r="C36" t="str">
-        <f t="shared" ref="C36:C92" si="5">CHAR(B36)</f>
+        <f t="shared" ref="C36:C99" si="5">CHAR(B36)</f>
         <v>B</v>
       </c>
       <c r="D36" t="s">
@@ -1711,7 +1717,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>43B61C</v>
@@ -1743,7 +1749,7 @@
         <v>43B65C</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>43B620</v>
@@ -1771,7 +1777,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>43B624</v>
@@ -1789,7 +1795,7 @@
       <c r="E39" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="2" t="s">
         <v>62</v>
       </c>
       <c r="G39" s="2" t="s">
@@ -1799,7 +1805,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>43B628</v>
@@ -1827,9 +1833,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX((B41 - 32)*4+HEX2DEC($M$1))</f>
         <v>43B62C</v>
       </c>
       <c r="B41">
@@ -1845,8 +1851,8 @@
       <c r="E41" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F41" t="s">
-        <v>64</v>
+      <c r="F41" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="G41" t="s">
         <v>57</v>
@@ -1855,7 +1861,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>43B630</v>
@@ -1883,7 +1889,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>43B634</v>
@@ -1901,8 +1907,8 @@
       <c r="E43" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F43" t="s">
-        <v>81</v>
+      <c r="F43" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="G43" t="s">
         <v>57</v>
@@ -1911,7 +1917,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>43B638</v>
@@ -1930,7 +1936,7 @@
         <v>11</v>
       </c>
       <c r="F44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G44" t="s">
         <v>57</v>
@@ -1939,7 +1945,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>43B63C</v>
@@ -1967,7 +1973,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>43B640</v>
@@ -1982,11 +1988,11 @@
       <c r="D46" t="s">
         <v>11</v>
       </c>
-      <c r="E46" s="4">
-        <v>11</v>
-      </c>
-      <c r="F46" t="s">
-        <v>84</v>
+      <c r="E46" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="G46" t="s">
         <v>57</v>
@@ -1995,7 +2001,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>43B644</v>
@@ -2016,14 +2022,14 @@
       <c r="F47" t="s">
         <v>63</v>
       </c>
-      <c r="G47" t="s">
-        <v>57</v>
+      <c r="G47" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>43B648</v>
@@ -2051,7 +2057,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>43B64C</v>
@@ -2070,16 +2076,16 @@
         <v>10</v>
       </c>
       <c r="F49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>43B650</v>
@@ -2107,7 +2113,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>43B654</v>
@@ -2135,7 +2141,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>43B658</v>
@@ -2153,8 +2159,8 @@
       <c r="E52" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F52" t="s">
-        <v>63</v>
+      <c r="F52" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="G52" t="s">
         <v>57</v>
@@ -2163,7 +2169,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="str">
         <f>DEC2HEX((B53 - 32)*4+HEX2DEC($M$1))</f>
         <v>43B65C</v>
@@ -2181,7 +2187,7 @@
       <c r="E53" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="2" t="s">
         <v>62</v>
       </c>
       <c r="G53" s="2" t="s">
@@ -2191,7 +2197,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>43B660</v>
@@ -2219,7 +2225,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>43B664</v>
@@ -2247,7 +2253,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="str">
         <f t="shared" si="0"/>
         <v>43B668</v>
@@ -2275,7 +2281,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="str">
         <f t="shared" si="0"/>
         <v>43B66C</v>
@@ -2290,11 +2296,11 @@
       <c r="D57" t="s">
         <v>22</v>
       </c>
-      <c r="E57" s="4">
-        <v>12</v>
-      </c>
-      <c r="F57" t="s">
-        <v>82</v>
+      <c r="E57" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="G57" t="s">
         <v>57</v>
@@ -2303,7 +2309,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="str">
         <f t="shared" si="0"/>
         <v>43B670</v>
@@ -2318,11 +2324,11 @@
       <c r="D58" t="s">
         <v>23</v>
       </c>
-      <c r="E58" s="4">
-        <v>12</v>
-      </c>
-      <c r="F58" t="s">
-        <v>82</v>
+      <c r="E58" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="G58" t="s">
         <v>57</v>
@@ -2331,7 +2337,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="str">
         <f t="shared" si="0"/>
         <v>43B674</v>
@@ -2346,11 +2352,11 @@
       <c r="D59" t="s">
         <v>24</v>
       </c>
-      <c r="E59" s="4">
-        <v>12</v>
-      </c>
-      <c r="F59" t="s">
-        <v>82</v>
+      <c r="E59" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="G59" t="s">
         <v>57</v>
@@ -2359,7 +2365,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="str">
         <f t="shared" si="0"/>
         <v>43B678</v>
@@ -2374,11 +2380,11 @@
       <c r="D60" t="s">
         <v>25</v>
       </c>
-      <c r="E60" s="4">
-        <v>12</v>
-      </c>
-      <c r="F60" t="s">
-        <v>82</v>
+      <c r="E60" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="G60" t="s">
         <v>57</v>
@@ -2387,7 +2393,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="str">
         <f t="shared" si="0"/>
         <v>43B67C</v>
@@ -2412,7 +2418,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="str">
         <f t="shared" si="0"/>
         <v>43B680</v>
@@ -2437,7 +2443,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="str">
         <f t="shared" si="0"/>
         <v>43B684</v>
@@ -2462,7 +2468,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="str">
         <f t="shared" si="0"/>
         <v>43B688</v>
@@ -2487,7 +2493,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" t="str">
         <f t="shared" si="0"/>
         <v>43B68C</v>
@@ -2512,9 +2518,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" t="str">
-        <f t="shared" ref="A66:A92" si="6">DEC2HEX((B66 - 32)*4+HEX2DEC($M$1))</f>
+        <f t="shared" ref="A66:A104" si="6">DEC2HEX((B66 - 32)*4+HEX2DEC($M$1))</f>
         <v>43B690</v>
       </c>
       <c r="B66">
@@ -2537,7 +2543,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" t="str">
         <f t="shared" si="6"/>
         <v>43B694</v>
@@ -2553,10 +2559,10 @@
         <v>26</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F67" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>62</v>
@@ -2565,7 +2571,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" t="str">
         <f t="shared" si="6"/>
         <v>43B698</v>
@@ -2593,7 +2599,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" t="str">
         <f>DEC2HEX((B69 - 32)*4+HEX2DEC($M$1))</f>
         <v>43B69C</v>
@@ -2609,7 +2615,7 @@
         <v>28</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>76</v>
@@ -2621,7 +2627,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" t="str">
         <f t="shared" si="6"/>
         <v>43B6A0</v>
@@ -2649,7 +2655,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" t="str">
         <f t="shared" si="6"/>
         <v>43B6A4</v>
@@ -2665,7 +2671,7 @@
         <v>30</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>76</v>
@@ -2677,7 +2683,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" t="str">
         <f t="shared" si="6"/>
         <v>43B6A8</v>
@@ -2692,11 +2698,11 @@
       <c r="D72" t="s">
         <v>31</v>
       </c>
-      <c r="E72" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F72" t="s">
-        <v>80</v>
+      <c r="E72" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="G72" t="s">
         <v>57</v>
@@ -2706,7 +2712,7 @@
       </c>
       <c r="J72" s="4"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" t="str">
         <f t="shared" si="6"/>
         <v>43B6AC</v>
@@ -2734,7 +2740,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" t="str">
         <f t="shared" si="6"/>
         <v>43B6B0</v>
@@ -2762,7 +2768,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" t="str">
         <f t="shared" si="6"/>
         <v>43B6B4</v>
@@ -2780,8 +2786,8 @@
       <c r="E75" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="F75" t="s">
-        <v>75</v>
+      <c r="F75" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>75</v>
@@ -2790,7 +2796,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" t="str">
         <f t="shared" si="6"/>
         <v>43B6B8</v>
@@ -2805,11 +2811,11 @@
       <c r="D76" t="s">
         <v>35</v>
       </c>
-      <c r="E76" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F76" t="s">
-        <v>80</v>
+      <c r="E76" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="G76" t="s">
         <v>57</v>
@@ -2818,7 +2824,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" t="str">
         <f t="shared" si="6"/>
         <v>43B6BC</v>
@@ -2836,8 +2842,8 @@
       <c r="E77" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F77" t="s">
-        <v>80</v>
+      <c r="F77" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="G77" t="s">
         <v>57</v>
@@ -2847,7 +2853,7 @@
       </c>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" t="str">
         <f t="shared" si="6"/>
         <v>43B6C0</v>
@@ -2863,10 +2869,10 @@
         <v>37</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>75</v>
@@ -2875,7 +2881,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" t="str">
         <f t="shared" si="6"/>
         <v>43B6C4</v>
@@ -2897,13 +2903,13 @@
         <v>63</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H79" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" t="str">
         <f t="shared" si="6"/>
         <v>43B6C8</v>
@@ -2919,10 +2925,10 @@
         <v>39</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G80" t="s">
         <v>57</v>
@@ -2931,7 +2937,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="str">
         <f t="shared" si="6"/>
         <v>43B6CC</v>
@@ -2959,7 +2965,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="str">
         <f t="shared" si="6"/>
         <v>43B6D0</v>
@@ -2977,17 +2983,17 @@
       <c r="E82" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F82" t="s">
-        <v>80</v>
-      </c>
-      <c r="G82" t="s">
-        <v>57</v>
+      <c r="F82" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="H82" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" t="str">
         <f t="shared" si="6"/>
         <v>43B6D4</v>
@@ -3015,7 +3021,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="str">
         <f t="shared" si="6"/>
         <v>43B6D8</v>
@@ -3033,8 +3039,8 @@
       <c r="E84" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F84">
-        <v>7</v>
+      <c r="F84" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>79</v>
@@ -3043,7 +3049,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" t="str">
         <f t="shared" si="6"/>
         <v>43B6DC</v>
@@ -3061,8 +3067,8 @@
       <c r="E85" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F85" t="s">
-        <v>80</v>
+      <c r="F85" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="G85" t="s">
         <v>57</v>
@@ -3071,7 +3077,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" t="str">
         <f t="shared" si="6"/>
         <v>43B6E0</v>
@@ -3089,8 +3095,8 @@
       <c r="E86" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F86" t="s">
-        <v>76</v>
+      <c r="F86" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="G86" t="s">
         <v>57</v>
@@ -3099,7 +3105,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" t="str">
         <f t="shared" si="6"/>
         <v>43B6E4</v>
@@ -3127,7 +3133,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" t="str">
         <f t="shared" si="6"/>
         <v>43B6E8</v>
@@ -3145,8 +3151,8 @@
       <c r="E88" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F88" t="s">
-        <v>80</v>
+      <c r="F88" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="G88" t="s">
         <v>57</v>
@@ -3155,7 +3161,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" t="str">
         <f t="shared" si="6"/>
         <v>43B6EC</v>
@@ -3183,7 +3189,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" t="str">
         <f t="shared" si="6"/>
         <v>43B6F0</v>
@@ -3201,8 +3207,8 @@
       <c r="E90" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F90" t="s">
-        <v>80</v>
+      <c r="F90" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="G90" t="s">
         <v>57</v>
@@ -3211,7 +3217,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="str">
         <f t="shared" si="6"/>
         <v>43B6F4</v>
@@ -3239,7 +3245,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="str">
         <f t="shared" si="6"/>
         <v>43B6F8</v>
@@ -3267,7 +3273,411 @@
         <v>72</v>
       </c>
     </row>
-    <row r="114" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A93" t="str">
+        <f t="shared" si="6"/>
+        <v>43B6FC</v>
+      </c>
+      <c r="B93">
+        <v>123</v>
+      </c>
+      <c r="C93" t="str">
+        <f t="shared" si="5"/>
+        <v>{</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F93" t="s">
+        <v>80</v>
+      </c>
+      <c r="G93" t="s">
+        <v>57</v>
+      </c>
+      <c r="H93" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A94" t="str">
+        <f t="shared" si="6"/>
+        <v>43B700</v>
+      </c>
+      <c r="B94">
+        <v>124</v>
+      </c>
+      <c r="C94" t="str">
+        <f t="shared" si="5"/>
+        <v>|</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F94" t="s">
+        <v>80</v>
+      </c>
+      <c r="G94" t="s">
+        <v>57</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A95" t="str">
+        <f t="shared" si="6"/>
+        <v>43B704</v>
+      </c>
+      <c r="B95">
+        <v>125</v>
+      </c>
+      <c r="C95" t="str">
+        <f t="shared" si="5"/>
+        <v>}</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F95" t="s">
+        <v>80</v>
+      </c>
+      <c r="G95" t="s">
+        <v>57</v>
+      </c>
+      <c r="H95" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A96" t="str">
+        <f t="shared" si="6"/>
+        <v>43B708</v>
+      </c>
+      <c r="B96">
+        <v>126</v>
+      </c>
+      <c r="C96" t="str">
+        <f t="shared" si="5"/>
+        <v>~</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F96" t="s">
+        <v>80</v>
+      </c>
+      <c r="G96" t="s">
+        <v>57</v>
+      </c>
+      <c r="H96" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A97" t="str">
+        <f t="shared" si="6"/>
+        <v>43B70C</v>
+      </c>
+      <c r="B97">
+        <v>127</v>
+      </c>
+      <c r="C97" t="s">
+        <v>86</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F97" t="s">
+        <v>80</v>
+      </c>
+      <c r="G97" t="s">
+        <v>57</v>
+      </c>
+      <c r="H97" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A98" t="str">
+        <f t="shared" si="6"/>
+        <v>43B710</v>
+      </c>
+      <c r="B98">
+        <v>128</v>
+      </c>
+      <c r="C98" t="str">
+        <f t="shared" si="5"/>
+        <v>€</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F98" t="s">
+        <v>80</v>
+      </c>
+      <c r="G98" t="s">
+        <v>57</v>
+      </c>
+      <c r="H98" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A99" t="str">
+        <f t="shared" si="6"/>
+        <v>43B714</v>
+      </c>
+      <c r="B99">
+        <v>129</v>
+      </c>
+      <c r="C99" t="str">
+        <f t="shared" si="5"/>
+        <v></v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F99" t="s">
+        <v>80</v>
+      </c>
+      <c r="G99" t="s">
+        <v>57</v>
+      </c>
+      <c r="H99" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A100" t="str">
+        <f t="shared" si="6"/>
+        <v>43B718</v>
+      </c>
+      <c r="B100">
+        <v>130</v>
+      </c>
+      <c r="C100" t="str">
+        <f t="shared" ref="C100:C109" si="7">CHAR(B100)</f>
+        <v>‚</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F100" t="s">
+        <v>80</v>
+      </c>
+      <c r="G100" t="s">
+        <v>57</v>
+      </c>
+      <c r="H100" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A101" t="str">
+        <f t="shared" si="6"/>
+        <v>43B71C</v>
+      </c>
+      <c r="B101">
+        <v>131</v>
+      </c>
+      <c r="C101" t="str">
+        <f t="shared" si="7"/>
+        <v>ƒ</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F101" t="s">
+        <v>80</v>
+      </c>
+      <c r="G101" t="s">
+        <v>57</v>
+      </c>
+      <c r="H101" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A102" t="str">
+        <f t="shared" si="6"/>
+        <v>43B720</v>
+      </c>
+      <c r="B102">
+        <v>132</v>
+      </c>
+      <c r="C102" t="str">
+        <f t="shared" si="7"/>
+        <v>„</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F102" t="s">
+        <v>80</v>
+      </c>
+      <c r="G102" t="s">
+        <v>57</v>
+      </c>
+      <c r="H102" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A103" t="str">
+        <f t="shared" si="6"/>
+        <v>43B724</v>
+      </c>
+      <c r="B103">
+        <v>133</v>
+      </c>
+      <c r="C103" t="str">
+        <f t="shared" si="7"/>
+        <v>…</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F103" t="s">
+        <v>80</v>
+      </c>
+      <c r="G103" t="s">
+        <v>57</v>
+      </c>
+      <c r="H103" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A104" t="str">
+        <f t="shared" si="6"/>
+        <v>43B728</v>
+      </c>
+      <c r="B104">
+        <v>134</v>
+      </c>
+      <c r="C104" t="str">
+        <f t="shared" si="7"/>
+        <v>†</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F104" t="s">
+        <v>80</v>
+      </c>
+      <c r="G104" t="s">
+        <v>57</v>
+      </c>
+      <c r="H104" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B105">
+        <v>135</v>
+      </c>
+      <c r="C105" t="str">
+        <f t="shared" si="7"/>
+        <v>‡</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F105" t="s">
+        <v>80</v>
+      </c>
+      <c r="G105" t="s">
+        <v>57</v>
+      </c>
+      <c r="H105" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B106">
+        <v>136</v>
+      </c>
+      <c r="C106" t="str">
+        <f t="shared" si="7"/>
+        <v>ˆ</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F106" t="s">
+        <v>80</v>
+      </c>
+      <c r="G106" t="s">
+        <v>57</v>
+      </c>
+      <c r="H106" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B107">
+        <v>137</v>
+      </c>
+      <c r="C107" t="str">
+        <f t="shared" si="7"/>
+        <v>‰</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F107" t="s">
+        <v>80</v>
+      </c>
+      <c r="G107" t="s">
+        <v>57</v>
+      </c>
+      <c r="H107" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B108">
+        <v>138</v>
+      </c>
+      <c r="C108" t="str">
+        <f t="shared" si="7"/>
+        <v>Š</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F108" t="s">
+        <v>80</v>
+      </c>
+      <c r="G108" t="s">
+        <v>57</v>
+      </c>
+      <c r="H108" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B109">
+        <v>139</v>
+      </c>
+      <c r="C109" t="str">
+        <f t="shared" si="7"/>
+        <v>‹</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F109" t="s">
+        <v>80</v>
+      </c>
+      <c r="G109" t="s">
+        <v>57</v>
+      </c>
+      <c r="H109" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="114" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K114" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Update font and fix characters with 0x3F
</commit_message>
<xml_diff>
--- a/2_translated/font/VWF_Properties.xlsx
+++ b/2_translated/font/VWF_Properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forti\Documents\GitHub\Super-Robot-Wars-Z\2_translated\font\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1934B8BA-6B0E-4006-BAB3-3D57ED7D4E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81AB3B9-193A-4C17-8E5A-EB49344691C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{4CE9F589-6C49-444B-92C3-C90A26708452}"/>
   </bookViews>
@@ -687,8 +687,8 @@
   <dimension ref="A1:M114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -758,6 +758,10 @@
       <c r="H2" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I2" t="str">
+        <f>DEC2HEX(B2)</f>
+        <v>20</v>
+      </c>
       <c r="L2" s="1"/>
       <c r="M2" s="2"/>
     </row>
@@ -777,14 +781,18 @@
       <c r="E3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F3" t="s">
-        <v>65</v>
+      <c r="F3" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="G3" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>68</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I66" si="2">DEC2HEX(B3)</f>
+        <v>21</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="2"/>
@@ -814,6 +822,10 @@
       <c r="H4" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I4" t="str">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
       <c r="L4" s="1"/>
       <c r="M4" s="2"/>
     </row>
@@ -826,7 +838,7 @@
         <v>35</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" ref="C5:C10" si="2">CHAR(B5)</f>
+        <f t="shared" ref="C5:C10" si="3">CHAR(B5)</f>
         <v>#</v>
       </c>
       <c r="D5" s="1"/>
@@ -842,6 +854,10 @@
       <c r="H5" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I5" t="str">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
       <c r="L5" s="1"/>
       <c r="M5" s="2"/>
     </row>
@@ -854,7 +870,7 @@
         <v>36</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>$</v>
       </c>
       <c r="D6" s="1"/>
@@ -870,6 +886,10 @@
       <c r="H6" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I6" t="str">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
       <c r="L6" s="1"/>
       <c r="M6" s="2"/>
     </row>
@@ -882,7 +902,7 @@
         <v>37</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>%</v>
       </c>
       <c r="D7" s="1"/>
@@ -898,6 +918,10 @@
       <c r="H7" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I7" t="str">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
       <c r="L7" s="1"/>
       <c r="M7" s="2"/>
     </row>
@@ -910,7 +934,7 @@
         <v>38</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>&amp;</v>
       </c>
       <c r="D8" s="1"/>
@@ -926,6 +950,10 @@
       <c r="H8" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I8" t="str">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
       <c r="L8" s="1"/>
       <c r="M8" s="2"/>
     </row>
@@ -938,7 +966,7 @@
         <v>39</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>'</v>
       </c>
       <c r="D9" s="1"/>
@@ -954,6 +982,10 @@
       <c r="H9" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I9" t="str">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
       <c r="L9" s="1"/>
       <c r="M9" s="2"/>
     </row>
@@ -966,21 +998,25 @@
         <v>40</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" t="s">
-        <v>65</v>
+      <c r="E10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="G10" t="s">
         <v>57</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>68</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="2"/>
+        <v>28</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="2"/>
@@ -994,21 +1030,25 @@
         <v>41</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" ref="C11:C16" si="3">CHAR(B11)</f>
+        <f t="shared" ref="C11:C16" si="4">CHAR(B11)</f>
         <v>)</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F11" t="s">
-        <v>65</v>
+      <c r="E11" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="G11" t="s">
         <v>57</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>68</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="2"/>
+        <v>29</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="2"/>
@@ -1022,7 +1062,7 @@
         <v>42</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>*</v>
       </c>
       <c r="D12" s="1"/>
@@ -1038,6 +1078,10 @@
       <c r="H12" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I12" t="str">
+        <f t="shared" si="2"/>
+        <v>2A</v>
+      </c>
       <c r="L12" s="1"/>
       <c r="M12" s="2"/>
     </row>
@@ -1050,7 +1094,7 @@
         <v>43</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>+</v>
       </c>
       <c r="D13" s="1"/>
@@ -1066,6 +1110,10 @@
       <c r="H13" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I13" t="str">
+        <f t="shared" si="2"/>
+        <v>2B</v>
+      </c>
       <c r="L13" s="1"/>
       <c r="M13" s="2"/>
     </row>
@@ -1078,7 +1126,7 @@
         <v>44</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="D14" s="1"/>
@@ -1094,6 +1142,10 @@
       <c r="H14" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I14" t="str">
+        <f t="shared" si="2"/>
+        <v>2C</v>
+      </c>
       <c r="L14" s="1"/>
       <c r="M14" s="2"/>
     </row>
@@ -1106,7 +1158,7 @@
         <v>45</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="D15" s="1"/>
@@ -1122,6 +1174,10 @@
       <c r="H15" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I15" t="str">
+        <f t="shared" si="2"/>
+        <v>2D</v>
+      </c>
       <c r="L15" s="1"/>
       <c r="M15" s="2"/>
     </row>
@@ -1134,7 +1190,7 @@
         <v>46</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="D16" s="1"/>
@@ -1150,6 +1206,10 @@
       <c r="H16" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I16" t="str">
+        <f t="shared" si="2"/>
+        <v>2E</v>
+      </c>
       <c r="L16" s="1"/>
       <c r="M16" s="2"/>
     </row>
@@ -1162,7 +1222,7 @@
         <v>47</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" ref="C17:C34" si="4">CHAR(B17)</f>
+        <f t="shared" ref="C17:C34" si="5">CHAR(B17)</f>
         <v>/</v>
       </c>
       <c r="D17" s="1"/>
@@ -1178,6 +1238,10 @@
       <c r="H17" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I17" t="str">
+        <f t="shared" si="2"/>
+        <v>2F</v>
+      </c>
       <c r="L17" s="1"/>
       <c r="M17" s="2"/>
     </row>
@@ -1190,7 +1254,7 @@
         <v>48</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D18" s="1"/>
@@ -1206,6 +1270,10 @@
       <c r="H18" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I18" t="str">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
       <c r="L18" s="1"/>
       <c r="M18" s="2"/>
     </row>
@@ -1218,7 +1286,7 @@
         <v>49</v>
       </c>
       <c r="C19" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="D19" s="1"/>
@@ -1234,6 +1302,10 @@
       <c r="H19" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I19" t="str">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
       <c r="L19" s="1"/>
       <c r="M19" s="2"/>
     </row>
@@ -1246,7 +1318,7 @@
         <v>50</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="D20" s="1"/>
@@ -1262,6 +1334,10 @@
       <c r="H20" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I20" t="str">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
       <c r="L20" s="1"/>
       <c r="M20" s="2"/>
     </row>
@@ -1274,7 +1350,7 @@
         <v>51</v>
       </c>
       <c r="C21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="D21" s="1"/>
@@ -1290,6 +1366,10 @@
       <c r="H21" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I21" t="str">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
       <c r="L21" s="1"/>
       <c r="M21" s="2"/>
     </row>
@@ -1302,7 +1382,7 @@
         <v>52</v>
       </c>
       <c r="C22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="D22" s="1"/>
@@ -1318,6 +1398,10 @@
       <c r="H22" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I22" t="str">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
       <c r="L22" s="1"/>
       <c r="M22" s="2"/>
     </row>
@@ -1330,7 +1414,7 @@
         <v>53</v>
       </c>
       <c r="C23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="D23" s="1"/>
@@ -1346,6 +1430,10 @@
       <c r="H23" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I23" t="str">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
       <c r="L23" s="1"/>
       <c r="M23" s="2"/>
     </row>
@@ -1358,7 +1446,7 @@
         <v>54</v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="D24" s="1"/>
@@ -1374,6 +1462,10 @@
       <c r="H24" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I24" t="str">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
       <c r="L24" s="1"/>
       <c r="M24" s="2"/>
     </row>
@@ -1386,7 +1478,7 @@
         <v>55</v>
       </c>
       <c r="C25" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="D25" s="1"/>
@@ -1402,6 +1494,10 @@
       <c r="H25" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I25" t="str">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
       <c r="L25" s="1"/>
       <c r="M25" s="2"/>
     </row>
@@ -1414,7 +1510,7 @@
         <v>56</v>
       </c>
       <c r="C26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="D26" s="1"/>
@@ -1430,6 +1526,10 @@
       <c r="H26" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I26" t="str">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
       <c r="L26" s="1"/>
       <c r="M26" s="2"/>
     </row>
@@ -1442,7 +1542,7 @@
         <v>57</v>
       </c>
       <c r="C27" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="D27" s="1"/>
@@ -1458,6 +1558,10 @@
       <c r="H27" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I27" t="str">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
       <c r="L27" s="1"/>
       <c r="M27" s="2"/>
     </row>
@@ -1470,7 +1574,7 @@
         <v>58</v>
       </c>
       <c r="C28" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>:</v>
       </c>
       <c r="D28" s="1"/>
@@ -1486,6 +1590,10 @@
       <c r="H28" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I28" t="str">
+        <f t="shared" si="2"/>
+        <v>3A</v>
+      </c>
       <c r="L28" s="1"/>
       <c r="M28" s="2"/>
     </row>
@@ -1498,7 +1606,7 @@
         <v>59</v>
       </c>
       <c r="C29" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>;</v>
       </c>
       <c r="D29" s="1"/>
@@ -1514,6 +1622,10 @@
       <c r="H29" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I29" t="str">
+        <f t="shared" si="2"/>
+        <v>3B</v>
+      </c>
       <c r="L29" s="1"/>
       <c r="M29" s="2"/>
     </row>
@@ -1526,7 +1638,7 @@
         <v>60</v>
       </c>
       <c r="C30" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;</v>
       </c>
       <c r="D30" s="1"/>
@@ -1542,6 +1654,10 @@
       <c r="H30" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I30" t="str">
+        <f t="shared" si="2"/>
+        <v>3C</v>
+      </c>
       <c r="L30" s="1"/>
       <c r="M30" s="2"/>
     </row>
@@ -1554,7 +1670,7 @@
         <v>61</v>
       </c>
       <c r="C31" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>=</v>
       </c>
       <c r="D31" s="1"/>
@@ -1570,6 +1686,10 @@
       <c r="H31" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I31" t="str">
+        <f t="shared" si="2"/>
+        <v>3D</v>
+      </c>
       <c r="L31" s="1"/>
       <c r="M31" s="2"/>
     </row>
@@ -1582,7 +1702,7 @@
         <v>62</v>
       </c>
       <c r="C32" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&gt;</v>
       </c>
       <c r="D32" s="1"/>
@@ -1598,6 +1718,10 @@
       <c r="H32" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I32" t="str">
+        <f t="shared" si="2"/>
+        <v>3E</v>
+      </c>
       <c r="L32" s="1"/>
       <c r="M32" s="2"/>
     </row>
@@ -1610,7 +1734,7 @@
         <v>63</v>
       </c>
       <c r="C33" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>?</v>
       </c>
       <c r="D33" s="1"/>
@@ -1626,6 +1750,10 @@
       <c r="H33" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I33" t="str">
+        <f t="shared" si="2"/>
+        <v>3F</v>
+      </c>
       <c r="L33" s="1"/>
       <c r="M33" s="2"/>
     </row>
@@ -1638,7 +1766,7 @@
         <v>64</v>
       </c>
       <c r="C34" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>@</v>
       </c>
       <c r="D34" s="1"/>
@@ -1653,6 +1781,10 @@
       </c>
       <c r="H34" s="4" t="s">
         <v>68</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="2"/>
+        <v>40</v>
       </c>
       <c r="L34" s="1"/>
       <c r="M34" s="2"/>
@@ -1684,6 +1816,10 @@
       <c r="H35" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="I35" t="str">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
       <c r="J35">
         <f>83-32</f>
         <v>51</v>
@@ -1698,7 +1834,7 @@
         <v>66</v>
       </c>
       <c r="C36" t="str">
-        <f t="shared" ref="C36:C99" si="5">CHAR(B36)</f>
+        <f t="shared" ref="C36:C99" si="6">CHAR(B36)</f>
         <v>B</v>
       </c>
       <c r="D36" t="s">
@@ -1716,6 +1852,10 @@
       <c r="H36" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I36" t="str">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="str">
@@ -1726,7 +1866,7 @@
         <v>67</v>
       </c>
       <c r="C37" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>C</v>
       </c>
       <c r="D37" t="s">
@@ -1743,6 +1883,10 @@
       </c>
       <c r="H37" s="4" t="s">
         <v>69</v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="2"/>
+        <v>43</v>
       </c>
       <c r="J37" t="str">
         <f>DEC2HEX(HEX2DEC($M$1)+4*J35)</f>
@@ -1758,7 +1902,7 @@
         <v>68</v>
       </c>
       <c r="C38" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>D</v>
       </c>
       <c r="D38" t="s">
@@ -1776,6 +1920,10 @@
       <c r="H38" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I38" t="str">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="str">
@@ -1786,7 +1934,7 @@
         <v>69</v>
       </c>
       <c r="C39" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="D39" t="s">
@@ -1804,6 +1952,10 @@
       <c r="H39" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I39" t="str">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" t="str">
@@ -1814,7 +1966,7 @@
         <v>70</v>
       </c>
       <c r="C40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>F</v>
       </c>
       <c r="D40" t="s">
@@ -1831,6 +1983,10 @@
       </c>
       <c r="H40" s="4" t="s">
         <v>70</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="2"/>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
@@ -1842,7 +1998,7 @@
         <v>71</v>
       </c>
       <c r="C41" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>G</v>
       </c>
       <c r="D41" t="s">
@@ -1860,6 +2016,10 @@
       <c r="H41" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="I41" t="str">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" t="str">
@@ -1870,7 +2030,7 @@
         <v>72</v>
       </c>
       <c r="C42" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>H</v>
       </c>
       <c r="D42" t="s">
@@ -1888,6 +2048,10 @@
       <c r="H42" s="4" t="s">
         <v>69</v>
       </c>
+      <c r="I42" t="str">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" t="str">
@@ -1898,7 +2062,7 @@
         <v>73</v>
       </c>
       <c r="C43" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>I</v>
       </c>
       <c r="D43" t="s">
@@ -1916,6 +2080,10 @@
       <c r="H43" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="I43" t="str">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" t="str">
@@ -1926,7 +2094,7 @@
         <v>74</v>
       </c>
       <c r="C44" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>J</v>
       </c>
       <c r="D44" t="s">
@@ -1944,6 +2112,10 @@
       <c r="H44" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="I44" t="str">
+        <f t="shared" si="2"/>
+        <v>4A</v>
+      </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" t="str">
@@ -1954,7 +2126,7 @@
         <v>75</v>
       </c>
       <c r="C45" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>K</v>
       </c>
       <c r="D45" t="s">
@@ -1972,6 +2144,10 @@
       <c r="H45" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I45" t="str">
+        <f t="shared" si="2"/>
+        <v>4B</v>
+      </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="str">
@@ -1982,7 +2158,7 @@
         <v>76</v>
       </c>
       <c r="C46" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>L</v>
       </c>
       <c r="D46" t="s">
@@ -2000,6 +2176,10 @@
       <c r="H46" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="I46" t="str">
+        <f t="shared" si="2"/>
+        <v>4C</v>
+      </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="str">
@@ -2010,7 +2190,7 @@
         <v>77</v>
       </c>
       <c r="C47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>M</v>
       </c>
       <c r="D47" t="s">
@@ -2028,6 +2208,10 @@
       <c r="H47" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="I47" t="str">
+        <f t="shared" si="2"/>
+        <v>4D</v>
+      </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" t="str">
@@ -2038,7 +2222,7 @@
         <v>78</v>
       </c>
       <c r="C48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>N</v>
       </c>
       <c r="D48" t="s">
@@ -2056,8 +2240,12 @@
       <c r="H48" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I48" t="str">
+        <f t="shared" si="2"/>
+        <v>4E</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>43B64C</v>
@@ -2066,7 +2254,7 @@
         <v>79</v>
       </c>
       <c r="C49" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>O</v>
       </c>
       <c r="D49" t="s">
@@ -2084,8 +2272,12 @@
       <c r="H49" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I49" t="str">
+        <f t="shared" si="2"/>
+        <v>4F</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>43B650</v>
@@ -2094,7 +2286,7 @@
         <v>80</v>
       </c>
       <c r="C50" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>P</v>
       </c>
       <c r="D50" t="s">
@@ -2112,8 +2304,12 @@
       <c r="H50" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I50" t="str">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>43B654</v>
@@ -2122,7 +2318,7 @@
         <v>81</v>
       </c>
       <c r="C51" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Q</v>
       </c>
       <c r="D51" t="s">
@@ -2140,8 +2336,12 @@
       <c r="H51" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I51" t="str">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>43B658</v>
@@ -2150,7 +2350,7 @@
         <v>82</v>
       </c>
       <c r="C52" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>R</v>
       </c>
       <c r="D52" t="s">
@@ -2168,8 +2368,12 @@
       <c r="H52" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I52" t="str">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="str">
         <f>DEC2HEX((B53 - 32)*4+HEX2DEC($M$1))</f>
         <v>43B65C</v>
@@ -2178,7 +2382,7 @@
         <v>83</v>
       </c>
       <c r="C53" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
       <c r="D53" t="s">
@@ -2196,8 +2400,12 @@
       <c r="H53" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I53" t="str">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>43B660</v>
@@ -2206,7 +2414,7 @@
         <v>84</v>
       </c>
       <c r="C54" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>T</v>
       </c>
       <c r="D54" t="s">
@@ -2224,8 +2432,12 @@
       <c r="H54" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I54" t="str">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>43B664</v>
@@ -2234,7 +2446,7 @@
         <v>85</v>
       </c>
       <c r="C55" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>U</v>
       </c>
       <c r="D55" t="s">
@@ -2252,8 +2464,12 @@
       <c r="H55" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I55" t="str">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="str">
         <f t="shared" si="0"/>
         <v>43B668</v>
@@ -2262,7 +2478,7 @@
         <v>86</v>
       </c>
       <c r="C56" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>V</v>
       </c>
       <c r="D56" t="s">
@@ -2280,8 +2496,12 @@
       <c r="H56" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I56" t="str">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="str">
         <f t="shared" si="0"/>
         <v>43B66C</v>
@@ -2290,7 +2510,7 @@
         <v>87</v>
       </c>
       <c r="C57" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>W</v>
       </c>
       <c r="D57" t="s">
@@ -2308,8 +2528,12 @@
       <c r="H57" s="4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I57" t="str">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="str">
         <f t="shared" si="0"/>
         <v>43B670</v>
@@ -2318,7 +2542,7 @@
         <v>88</v>
       </c>
       <c r="C58" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>X</v>
       </c>
       <c r="D58" t="s">
@@ -2336,8 +2560,12 @@
       <c r="H58" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I58" t="str">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="str">
         <f t="shared" si="0"/>
         <v>43B674</v>
@@ -2346,7 +2574,7 @@
         <v>89</v>
       </c>
       <c r="C59" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Y</v>
       </c>
       <c r="D59" t="s">
@@ -2364,8 +2592,12 @@
       <c r="H59" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I59" t="str">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="str">
         <f t="shared" si="0"/>
         <v>43B678</v>
@@ -2374,7 +2606,7 @@
         <v>90</v>
       </c>
       <c r="C60" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Z</v>
       </c>
       <c r="D60" t="s">
@@ -2392,8 +2624,12 @@
       <c r="H60" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I60" t="str">
+        <f t="shared" si="2"/>
+        <v>5A</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="str">
         <f t="shared" si="0"/>
         <v>43B67C</v>
@@ -2402,7 +2638,7 @@
         <v>91</v>
       </c>
       <c r="C61" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>[</v>
       </c>
       <c r="E61" s="4" t="s">
@@ -2417,8 +2653,12 @@
       <c r="H61" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I61" t="str">
+        <f t="shared" si="2"/>
+        <v>5B</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="str">
         <f t="shared" si="0"/>
         <v>43B680</v>
@@ -2427,7 +2667,7 @@
         <v>92</v>
       </c>
       <c r="C62" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>\</v>
       </c>
       <c r="E62" s="4" t="s">
@@ -2442,8 +2682,12 @@
       <c r="H62" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I62" t="str">
+        <f t="shared" si="2"/>
+        <v>5C</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="str">
         <f t="shared" si="0"/>
         <v>43B684</v>
@@ -2452,7 +2696,7 @@
         <v>93</v>
       </c>
       <c r="C63" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>]</v>
       </c>
       <c r="E63" s="4" t="s">
@@ -2467,8 +2711,12 @@
       <c r="H63" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I63" t="str">
+        <f t="shared" si="2"/>
+        <v>5D</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="str">
         <f t="shared" si="0"/>
         <v>43B688</v>
@@ -2477,7 +2725,7 @@
         <v>94</v>
       </c>
       <c r="C64" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>^</v>
       </c>
       <c r="E64" s="4" t="s">
@@ -2492,6 +2740,10 @@
       <c r="H64" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I64" t="str">
+        <f t="shared" si="2"/>
+        <v>5E</v>
+      </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" t="str">
@@ -2502,7 +2754,7 @@
         <v>95</v>
       </c>
       <c r="C65" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>_</v>
       </c>
       <c r="E65" s="4" t="s">
@@ -2517,17 +2769,21 @@
       <c r="H65" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I65" t="str">
+        <f t="shared" si="2"/>
+        <v>5F</v>
+      </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" t="str">
-        <f t="shared" ref="A66:A104" si="6">DEC2HEX((B66 - 32)*4+HEX2DEC($M$1))</f>
+        <f t="shared" ref="A66:A104" si="7">DEC2HEX((B66 - 32)*4+HEX2DEC($M$1))</f>
         <v>43B690</v>
       </c>
       <c r="B66">
         <v>96</v>
       </c>
       <c r="C66" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>`</v>
       </c>
       <c r="E66" s="4" t="s">
@@ -2542,17 +2798,21 @@
       <c r="H66" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I66" t="str">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B694</v>
       </c>
       <c r="B67">
         <v>97</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>a</v>
       </c>
       <c r="D67" t="s">
@@ -2570,17 +2830,21 @@
       <c r="H67" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="I67" t="str">
+        <f t="shared" ref="I67:I95" si="8">DEC2HEX(B67)</f>
+        <v>61</v>
+      </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B698</v>
       </c>
       <c r="B68">
         <v>98</v>
       </c>
       <c r="C68" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>b</v>
       </c>
       <c r="D68" t="s">
@@ -2597,6 +2861,10 @@
       </c>
       <c r="H68" s="4" t="s">
         <v>70</v>
+      </c>
+      <c r="I68" t="str">
+        <f t="shared" si="8"/>
+        <v>62</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.35">
@@ -2608,7 +2876,7 @@
         <v>99</v>
       </c>
       <c r="C69" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>c</v>
       </c>
       <c r="D69" t="s">
@@ -2626,17 +2894,21 @@
       <c r="H69" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="I69" t="str">
+        <f t="shared" si="8"/>
+        <v>63</v>
+      </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6A0</v>
       </c>
       <c r="B70">
         <v>100</v>
       </c>
       <c r="C70" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>d</v>
       </c>
       <c r="D70" t="s">
@@ -2654,17 +2926,21 @@
       <c r="H70" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I70" t="str">
+        <f t="shared" si="8"/>
+        <v>64</v>
+      </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6A4</v>
       </c>
       <c r="B71">
         <v>101</v>
       </c>
       <c r="C71" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>e</v>
       </c>
       <c r="D71" t="s">
@@ -2682,17 +2958,21 @@
       <c r="H71" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="I71" t="str">
+        <f t="shared" si="8"/>
+        <v>65</v>
+      </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6A8</v>
       </c>
       <c r="B72">
         <v>102</v>
       </c>
       <c r="C72" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>f</v>
       </c>
       <c r="D72" t="s">
@@ -2710,18 +2990,22 @@
       <c r="H72" s="4" t="s">
         <v>72</v>
       </c>
+      <c r="I72" t="str">
+        <f t="shared" si="8"/>
+        <v>66</v>
+      </c>
       <c r="J72" s="4"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6AC</v>
       </c>
       <c r="B73">
         <v>103</v>
       </c>
       <c r="C73" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>g</v>
       </c>
       <c r="D73" t="s">
@@ -2739,17 +3023,21 @@
       <c r="H73" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="I73" t="str">
+        <f t="shared" si="8"/>
+        <v>67</v>
+      </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6B0</v>
       </c>
       <c r="B74">
         <v>104</v>
       </c>
       <c r="C74" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>h</v>
       </c>
       <c r="D74" t="s">
@@ -2767,17 +3055,21 @@
       <c r="H74" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="I74" t="str">
+        <f t="shared" si="8"/>
+        <v>68</v>
+      </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6B4</v>
       </c>
       <c r="B75">
         <v>105</v>
       </c>
       <c r="C75" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>i</v>
       </c>
       <c r="D75" t="s">
@@ -2795,17 +3087,21 @@
       <c r="H75" s="4" t="s">
         <v>73</v>
       </c>
+      <c r="I75" t="str">
+        <f t="shared" si="8"/>
+        <v>69</v>
+      </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6B8</v>
       </c>
       <c r="B76">
         <v>106</v>
       </c>
       <c r="C76" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>j</v>
       </c>
       <c r="D76" t="s">
@@ -2823,17 +3119,21 @@
       <c r="H76" s="4" t="s">
         <v>72</v>
       </c>
+      <c r="I76" t="str">
+        <f t="shared" si="8"/>
+        <v>6A</v>
+      </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6BC</v>
       </c>
       <c r="B77">
         <v>107</v>
       </c>
       <c r="C77" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>k</v>
       </c>
       <c r="D77" t="s">
@@ -2851,18 +3151,22 @@
       <c r="H77" s="4" t="s">
         <v>72</v>
       </c>
+      <c r="I77" t="str">
+        <f t="shared" si="8"/>
+        <v>6B</v>
+      </c>
       <c r="L77" s="2"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6C0</v>
       </c>
       <c r="B78">
         <v>108</v>
       </c>
       <c r="C78" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>l</v>
       </c>
       <c r="D78" t="s">
@@ -2880,17 +3184,21 @@
       <c r="H78" s="4" t="s">
         <v>73</v>
       </c>
+      <c r="I78" t="str">
+        <f t="shared" si="8"/>
+        <v>6C</v>
+      </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6C4</v>
       </c>
       <c r="B79">
         <v>109</v>
       </c>
       <c r="C79" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>m</v>
       </c>
       <c r="D79" t="s">
@@ -2908,17 +3216,21 @@
       <c r="H79" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="I79" t="str">
+        <f t="shared" si="8"/>
+        <v>6D</v>
+      </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6C8</v>
       </c>
       <c r="B80">
         <v>110</v>
       </c>
       <c r="C80" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>n</v>
       </c>
       <c r="D80" t="s">
@@ -2936,17 +3248,21 @@
       <c r="H80" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I80" t="str">
+        <f t="shared" si="8"/>
+        <v>6E</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6CC</v>
       </c>
       <c r="B81">
         <v>111</v>
       </c>
       <c r="C81" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>o</v>
       </c>
       <c r="D81" t="s">
@@ -2964,17 +3280,21 @@
       <c r="H81" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I81" t="str">
+        <f t="shared" si="8"/>
+        <v>6F</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6D0</v>
       </c>
       <c r="B82">
         <v>112</v>
       </c>
       <c r="C82" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>p</v>
       </c>
       <c r="D82" t="s">
@@ -2992,17 +3312,21 @@
       <c r="H82" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I82" t="str">
+        <f t="shared" si="8"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6D4</v>
       </c>
       <c r="B83">
         <v>113</v>
       </c>
       <c r="C83" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>q</v>
       </c>
       <c r="D83" t="s">
@@ -3020,17 +3344,21 @@
       <c r="H83" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I83" t="str">
+        <f t="shared" si="8"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6D8</v>
       </c>
       <c r="B84">
         <v>114</v>
       </c>
       <c r="C84" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>r</v>
       </c>
       <c r="D84" t="s">
@@ -3048,17 +3376,21 @@
       <c r="H84" s="4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I84" t="str">
+        <f t="shared" si="8"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6DC</v>
       </c>
       <c r="B85">
         <v>115</v>
       </c>
       <c r="C85" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>s</v>
       </c>
       <c r="D85" t="s">
@@ -3076,17 +3408,21 @@
       <c r="H85" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I85" t="str">
+        <f t="shared" si="8"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6E0</v>
       </c>
       <c r="B86">
         <v>116</v>
       </c>
       <c r="C86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>t</v>
       </c>
       <c r="D86" t="s">
@@ -3104,17 +3440,21 @@
       <c r="H86" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I86" t="str">
+        <f t="shared" si="8"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6E4</v>
       </c>
       <c r="B87">
         <v>117</v>
       </c>
       <c r="C87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>u</v>
       </c>
       <c r="D87" t="s">
@@ -3132,17 +3472,21 @@
       <c r="H87" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I87" t="str">
+        <f t="shared" si="8"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6E8</v>
       </c>
       <c r="B88">
         <v>118</v>
       </c>
       <c r="C88" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>v</v>
       </c>
       <c r="D88" t="s">
@@ -3160,17 +3504,21 @@
       <c r="H88" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I88" t="str">
+        <f t="shared" si="8"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6EC</v>
       </c>
       <c r="B89">
         <v>119</v>
       </c>
       <c r="C89" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>w</v>
       </c>
       <c r="D89" t="s">
@@ -3188,17 +3536,21 @@
       <c r="H89" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I89" t="str">
+        <f t="shared" si="8"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6F0</v>
       </c>
       <c r="B90">
         <v>120</v>
       </c>
       <c r="C90" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>x</v>
       </c>
       <c r="D90" t="s">
@@ -3216,17 +3568,21 @@
       <c r="H90" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I90" t="str">
+        <f t="shared" si="8"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6F4</v>
       </c>
       <c r="B91">
         <v>121</v>
       </c>
       <c r="C91" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>y</v>
       </c>
       <c r="D91" t="s">
@@ -3244,17 +3600,21 @@
       <c r="H91" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I91" t="str">
+        <f t="shared" si="8"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6F8</v>
       </c>
       <c r="B92">
         <v>122</v>
       </c>
       <c r="C92" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>z</v>
       </c>
       <c r="D92" t="s">
@@ -3272,17 +3632,21 @@
       <c r="H92" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I92" t="str">
+        <f t="shared" si="8"/>
+        <v>7A</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6FC</v>
       </c>
       <c r="B93">
         <v>123</v>
       </c>
       <c r="C93" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>{</v>
       </c>
       <c r="E93" s="4" t="s">
@@ -3297,17 +3661,21 @@
       <c r="H93" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I93" t="str">
+        <f t="shared" si="8"/>
+        <v>7B</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B700</v>
       </c>
       <c r="B94">
         <v>124</v>
       </c>
       <c r="C94" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>|</v>
       </c>
       <c r="E94" s="4" t="s">
@@ -3322,17 +3690,21 @@
       <c r="H94" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I94" t="str">
+        <f t="shared" si="8"/>
+        <v>7C</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B704</v>
       </c>
       <c r="B95">
         <v>125</v>
       </c>
       <c r="C95" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>}</v>
       </c>
       <c r="E95" s="4" t="s">
@@ -3347,17 +3719,21 @@
       <c r="H95" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I95" t="str">
+        <f t="shared" si="8"/>
+        <v>7D</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B708</v>
       </c>
       <c r="B96">
         <v>126</v>
       </c>
       <c r="C96" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>~</v>
       </c>
       <c r="E96" s="4" t="s">
@@ -3375,7 +3751,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B70C</v>
       </c>
       <c r="B97">
@@ -3399,14 +3775,14 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B710</v>
       </c>
       <c r="B98">
         <v>128</v>
       </c>
       <c r="C98" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>€</v>
       </c>
       <c r="E98" s="4" t="s">
@@ -3424,14 +3800,14 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B714</v>
       </c>
       <c r="B99">
         <v>129</v>
       </c>
       <c r="C99" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v></v>
       </c>
       <c r="E99" s="4" t="s">
@@ -3449,14 +3825,14 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B718</v>
       </c>
       <c r="B100">
         <v>130</v>
       </c>
       <c r="C100" t="str">
-        <f t="shared" ref="C100:C109" si="7">CHAR(B100)</f>
+        <f t="shared" ref="C100:C109" si="9">CHAR(B100)</f>
         <v>‚</v>
       </c>
       <c r="E100" s="4" t="s">
@@ -3474,14 +3850,14 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B71C</v>
       </c>
       <c r="B101">
         <v>131</v>
       </c>
       <c r="C101" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>ƒ</v>
       </c>
       <c r="E101" s="4" t="s">
@@ -3499,14 +3875,14 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B720</v>
       </c>
       <c r="B102">
         <v>132</v>
       </c>
       <c r="C102" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>„</v>
       </c>
       <c r="E102" s="4" t="s">
@@ -3524,14 +3900,14 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B724</v>
       </c>
       <c r="B103">
         <v>133</v>
       </c>
       <c r="C103" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>…</v>
       </c>
       <c r="E103" s="4" t="s">
@@ -3549,14 +3925,14 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B728</v>
       </c>
       <c r="B104">
         <v>134</v>
       </c>
       <c r="C104" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>†</v>
       </c>
       <c r="E104" s="4" t="s">
@@ -3577,7 +3953,7 @@
         <v>135</v>
       </c>
       <c r="C105" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>‡</v>
       </c>
       <c r="E105" s="4" t="s">
@@ -3598,7 +3974,7 @@
         <v>136</v>
       </c>
       <c r="C106" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>ˆ</v>
       </c>
       <c r="E106" s="4" t="s">
@@ -3619,7 +3995,7 @@
         <v>137</v>
       </c>
       <c r="C107" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>‰</v>
       </c>
       <c r="E107" s="4" t="s">
@@ -3640,7 +4016,7 @@
         <v>138</v>
       </c>
       <c r="C108" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>Š</v>
       </c>
       <c r="E108" s="4" t="s">
@@ -3661,7 +4037,7 @@
         <v>139</v>
       </c>
       <c r="C109" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>‹</v>
       </c>
       <c r="E109" s="4" t="s">

</xml_diff>

<commit_message>
PR - Fix issue tlb miss breaking the game (#31)
* Fix issue with VT1.bin size and TLB miss crashing the game

* Update .gitignore

* Update font and fix characters with 0x3F
</commit_message>
<xml_diff>
--- a/2_translated/font/VWF_Properties.xlsx
+++ b/2_translated/font/VWF_Properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forti\Documents\GitHub\Super-Robot-Wars-Z\2_translated\font\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1934B8BA-6B0E-4006-BAB3-3D57ED7D4E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81AB3B9-193A-4C17-8E5A-EB49344691C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{4CE9F589-6C49-444B-92C3-C90A26708452}"/>
   </bookViews>
@@ -687,8 +687,8 @@
   <dimension ref="A1:M114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -758,6 +758,10 @@
       <c r="H2" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I2" t="str">
+        <f>DEC2HEX(B2)</f>
+        <v>20</v>
+      </c>
       <c r="L2" s="1"/>
       <c r="M2" s="2"/>
     </row>
@@ -777,14 +781,18 @@
       <c r="E3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F3" t="s">
-        <v>65</v>
+      <c r="F3" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="G3" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>68</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I66" si="2">DEC2HEX(B3)</f>
+        <v>21</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="2"/>
@@ -814,6 +822,10 @@
       <c r="H4" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I4" t="str">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
       <c r="L4" s="1"/>
       <c r="M4" s="2"/>
     </row>
@@ -826,7 +838,7 @@
         <v>35</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" ref="C5:C10" si="2">CHAR(B5)</f>
+        <f t="shared" ref="C5:C10" si="3">CHAR(B5)</f>
         <v>#</v>
       </c>
       <c r="D5" s="1"/>
@@ -842,6 +854,10 @@
       <c r="H5" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I5" t="str">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
       <c r="L5" s="1"/>
       <c r="M5" s="2"/>
     </row>
@@ -854,7 +870,7 @@
         <v>36</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>$</v>
       </c>
       <c r="D6" s="1"/>
@@ -870,6 +886,10 @@
       <c r="H6" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I6" t="str">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
       <c r="L6" s="1"/>
       <c r="M6" s="2"/>
     </row>
@@ -882,7 +902,7 @@
         <v>37</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>%</v>
       </c>
       <c r="D7" s="1"/>
@@ -898,6 +918,10 @@
       <c r="H7" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I7" t="str">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
       <c r="L7" s="1"/>
       <c r="M7" s="2"/>
     </row>
@@ -910,7 +934,7 @@
         <v>38</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>&amp;</v>
       </c>
       <c r="D8" s="1"/>
@@ -926,6 +950,10 @@
       <c r="H8" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I8" t="str">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
       <c r="L8" s="1"/>
       <c r="M8" s="2"/>
     </row>
@@ -938,7 +966,7 @@
         <v>39</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>'</v>
       </c>
       <c r="D9" s="1"/>
@@ -954,6 +982,10 @@
       <c r="H9" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I9" t="str">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
       <c r="L9" s="1"/>
       <c r="M9" s="2"/>
     </row>
@@ -966,21 +998,25 @@
         <v>40</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" t="s">
-        <v>65</v>
+      <c r="E10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="G10" t="s">
         <v>57</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>68</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="2"/>
+        <v>28</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="2"/>
@@ -994,21 +1030,25 @@
         <v>41</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" ref="C11:C16" si="3">CHAR(B11)</f>
+        <f t="shared" ref="C11:C16" si="4">CHAR(B11)</f>
         <v>)</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F11" t="s">
-        <v>65</v>
+      <c r="E11" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="G11" t="s">
         <v>57</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>68</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="2"/>
+        <v>29</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="2"/>
@@ -1022,7 +1062,7 @@
         <v>42</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>*</v>
       </c>
       <c r="D12" s="1"/>
@@ -1038,6 +1078,10 @@
       <c r="H12" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I12" t="str">
+        <f t="shared" si="2"/>
+        <v>2A</v>
+      </c>
       <c r="L12" s="1"/>
       <c r="M12" s="2"/>
     </row>
@@ -1050,7 +1094,7 @@
         <v>43</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>+</v>
       </c>
       <c r="D13" s="1"/>
@@ -1066,6 +1110,10 @@
       <c r="H13" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I13" t="str">
+        <f t="shared" si="2"/>
+        <v>2B</v>
+      </c>
       <c r="L13" s="1"/>
       <c r="M13" s="2"/>
     </row>
@@ -1078,7 +1126,7 @@
         <v>44</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="D14" s="1"/>
@@ -1094,6 +1142,10 @@
       <c r="H14" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I14" t="str">
+        <f t="shared" si="2"/>
+        <v>2C</v>
+      </c>
       <c r="L14" s="1"/>
       <c r="M14" s="2"/>
     </row>
@@ -1106,7 +1158,7 @@
         <v>45</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="D15" s="1"/>
@@ -1122,6 +1174,10 @@
       <c r="H15" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I15" t="str">
+        <f t="shared" si="2"/>
+        <v>2D</v>
+      </c>
       <c r="L15" s="1"/>
       <c r="M15" s="2"/>
     </row>
@@ -1134,7 +1190,7 @@
         <v>46</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="D16" s="1"/>
@@ -1150,6 +1206,10 @@
       <c r="H16" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I16" t="str">
+        <f t="shared" si="2"/>
+        <v>2E</v>
+      </c>
       <c r="L16" s="1"/>
       <c r="M16" s="2"/>
     </row>
@@ -1162,7 +1222,7 @@
         <v>47</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" ref="C17:C34" si="4">CHAR(B17)</f>
+        <f t="shared" ref="C17:C34" si="5">CHAR(B17)</f>
         <v>/</v>
       </c>
       <c r="D17" s="1"/>
@@ -1178,6 +1238,10 @@
       <c r="H17" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I17" t="str">
+        <f t="shared" si="2"/>
+        <v>2F</v>
+      </c>
       <c r="L17" s="1"/>
       <c r="M17" s="2"/>
     </row>
@@ -1190,7 +1254,7 @@
         <v>48</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D18" s="1"/>
@@ -1206,6 +1270,10 @@
       <c r="H18" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I18" t="str">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
       <c r="L18" s="1"/>
       <c r="M18" s="2"/>
     </row>
@@ -1218,7 +1286,7 @@
         <v>49</v>
       </c>
       <c r="C19" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="D19" s="1"/>
@@ -1234,6 +1302,10 @@
       <c r="H19" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I19" t="str">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
       <c r="L19" s="1"/>
       <c r="M19" s="2"/>
     </row>
@@ -1246,7 +1318,7 @@
         <v>50</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="D20" s="1"/>
@@ -1262,6 +1334,10 @@
       <c r="H20" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I20" t="str">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
       <c r="L20" s="1"/>
       <c r="M20" s="2"/>
     </row>
@@ -1274,7 +1350,7 @@
         <v>51</v>
       </c>
       <c r="C21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="D21" s="1"/>
@@ -1290,6 +1366,10 @@
       <c r="H21" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I21" t="str">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
       <c r="L21" s="1"/>
       <c r="M21" s="2"/>
     </row>
@@ -1302,7 +1382,7 @@
         <v>52</v>
       </c>
       <c r="C22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="D22" s="1"/>
@@ -1318,6 +1398,10 @@
       <c r="H22" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I22" t="str">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
       <c r="L22" s="1"/>
       <c r="M22" s="2"/>
     </row>
@@ -1330,7 +1414,7 @@
         <v>53</v>
       </c>
       <c r="C23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="D23" s="1"/>
@@ -1346,6 +1430,10 @@
       <c r="H23" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I23" t="str">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
       <c r="L23" s="1"/>
       <c r="M23" s="2"/>
     </row>
@@ -1358,7 +1446,7 @@
         <v>54</v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="D24" s="1"/>
@@ -1374,6 +1462,10 @@
       <c r="H24" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I24" t="str">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
       <c r="L24" s="1"/>
       <c r="M24" s="2"/>
     </row>
@@ -1386,7 +1478,7 @@
         <v>55</v>
       </c>
       <c r="C25" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="D25" s="1"/>
@@ -1402,6 +1494,10 @@
       <c r="H25" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I25" t="str">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
       <c r="L25" s="1"/>
       <c r="M25" s="2"/>
     </row>
@@ -1414,7 +1510,7 @@
         <v>56</v>
       </c>
       <c r="C26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="D26" s="1"/>
@@ -1430,6 +1526,10 @@
       <c r="H26" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I26" t="str">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
       <c r="L26" s="1"/>
       <c r="M26" s="2"/>
     </row>
@@ -1442,7 +1542,7 @@
         <v>57</v>
       </c>
       <c r="C27" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="D27" s="1"/>
@@ -1458,6 +1558,10 @@
       <c r="H27" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I27" t="str">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
       <c r="L27" s="1"/>
       <c r="M27" s="2"/>
     </row>
@@ -1470,7 +1574,7 @@
         <v>58</v>
       </c>
       <c r="C28" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>:</v>
       </c>
       <c r="D28" s="1"/>
@@ -1486,6 +1590,10 @@
       <c r="H28" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I28" t="str">
+        <f t="shared" si="2"/>
+        <v>3A</v>
+      </c>
       <c r="L28" s="1"/>
       <c r="M28" s="2"/>
     </row>
@@ -1498,7 +1606,7 @@
         <v>59</v>
       </c>
       <c r="C29" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>;</v>
       </c>
       <c r="D29" s="1"/>
@@ -1514,6 +1622,10 @@
       <c r="H29" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I29" t="str">
+        <f t="shared" si="2"/>
+        <v>3B</v>
+      </c>
       <c r="L29" s="1"/>
       <c r="M29" s="2"/>
     </row>
@@ -1526,7 +1638,7 @@
         <v>60</v>
       </c>
       <c r="C30" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;</v>
       </c>
       <c r="D30" s="1"/>
@@ -1542,6 +1654,10 @@
       <c r="H30" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I30" t="str">
+        <f t="shared" si="2"/>
+        <v>3C</v>
+      </c>
       <c r="L30" s="1"/>
       <c r="M30" s="2"/>
     </row>
@@ -1554,7 +1670,7 @@
         <v>61</v>
       </c>
       <c r="C31" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>=</v>
       </c>
       <c r="D31" s="1"/>
@@ -1570,6 +1686,10 @@
       <c r="H31" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I31" t="str">
+        <f t="shared" si="2"/>
+        <v>3D</v>
+      </c>
       <c r="L31" s="1"/>
       <c r="M31" s="2"/>
     </row>
@@ -1582,7 +1702,7 @@
         <v>62</v>
       </c>
       <c r="C32" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&gt;</v>
       </c>
       <c r="D32" s="1"/>
@@ -1598,6 +1718,10 @@
       <c r="H32" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I32" t="str">
+        <f t="shared" si="2"/>
+        <v>3E</v>
+      </c>
       <c r="L32" s="1"/>
       <c r="M32" s="2"/>
     </row>
@@ -1610,7 +1734,7 @@
         <v>63</v>
       </c>
       <c r="C33" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>?</v>
       </c>
       <c r="D33" s="1"/>
@@ -1626,6 +1750,10 @@
       <c r="H33" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I33" t="str">
+        <f t="shared" si="2"/>
+        <v>3F</v>
+      </c>
       <c r="L33" s="1"/>
       <c r="M33" s="2"/>
     </row>
@@ -1638,7 +1766,7 @@
         <v>64</v>
       </c>
       <c r="C34" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>@</v>
       </c>
       <c r="D34" s="1"/>
@@ -1653,6 +1781,10 @@
       </c>
       <c r="H34" s="4" t="s">
         <v>68</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="2"/>
+        <v>40</v>
       </c>
       <c r="L34" s="1"/>
       <c r="M34" s="2"/>
@@ -1684,6 +1816,10 @@
       <c r="H35" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="I35" t="str">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
       <c r="J35">
         <f>83-32</f>
         <v>51</v>
@@ -1698,7 +1834,7 @@
         <v>66</v>
       </c>
       <c r="C36" t="str">
-        <f t="shared" ref="C36:C99" si="5">CHAR(B36)</f>
+        <f t="shared" ref="C36:C99" si="6">CHAR(B36)</f>
         <v>B</v>
       </c>
       <c r="D36" t="s">
@@ -1716,6 +1852,10 @@
       <c r="H36" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I36" t="str">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="str">
@@ -1726,7 +1866,7 @@
         <v>67</v>
       </c>
       <c r="C37" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>C</v>
       </c>
       <c r="D37" t="s">
@@ -1743,6 +1883,10 @@
       </c>
       <c r="H37" s="4" t="s">
         <v>69</v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="2"/>
+        <v>43</v>
       </c>
       <c r="J37" t="str">
         <f>DEC2HEX(HEX2DEC($M$1)+4*J35)</f>
@@ -1758,7 +1902,7 @@
         <v>68</v>
       </c>
       <c r="C38" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>D</v>
       </c>
       <c r="D38" t="s">
@@ -1776,6 +1920,10 @@
       <c r="H38" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I38" t="str">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="str">
@@ -1786,7 +1934,7 @@
         <v>69</v>
       </c>
       <c r="C39" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="D39" t="s">
@@ -1804,6 +1952,10 @@
       <c r="H39" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I39" t="str">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" t="str">
@@ -1814,7 +1966,7 @@
         <v>70</v>
       </c>
       <c r="C40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>F</v>
       </c>
       <c r="D40" t="s">
@@ -1831,6 +1983,10 @@
       </c>
       <c r="H40" s="4" t="s">
         <v>70</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="2"/>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
@@ -1842,7 +1998,7 @@
         <v>71</v>
       </c>
       <c r="C41" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>G</v>
       </c>
       <c r="D41" t="s">
@@ -1860,6 +2016,10 @@
       <c r="H41" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="I41" t="str">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" t="str">
@@ -1870,7 +2030,7 @@
         <v>72</v>
       </c>
       <c r="C42" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>H</v>
       </c>
       <c r="D42" t="s">
@@ -1888,6 +2048,10 @@
       <c r="H42" s="4" t="s">
         <v>69</v>
       </c>
+      <c r="I42" t="str">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" t="str">
@@ -1898,7 +2062,7 @@
         <v>73</v>
       </c>
       <c r="C43" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>I</v>
       </c>
       <c r="D43" t="s">
@@ -1916,6 +2080,10 @@
       <c r="H43" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="I43" t="str">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" t="str">
@@ -1926,7 +2094,7 @@
         <v>74</v>
       </c>
       <c r="C44" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>J</v>
       </c>
       <c r="D44" t="s">
@@ -1944,6 +2112,10 @@
       <c r="H44" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="I44" t="str">
+        <f t="shared" si="2"/>
+        <v>4A</v>
+      </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" t="str">
@@ -1954,7 +2126,7 @@
         <v>75</v>
       </c>
       <c r="C45" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>K</v>
       </c>
       <c r="D45" t="s">
@@ -1972,6 +2144,10 @@
       <c r="H45" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I45" t="str">
+        <f t="shared" si="2"/>
+        <v>4B</v>
+      </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="str">
@@ -1982,7 +2158,7 @@
         <v>76</v>
       </c>
       <c r="C46" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>L</v>
       </c>
       <c r="D46" t="s">
@@ -2000,6 +2176,10 @@
       <c r="H46" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="I46" t="str">
+        <f t="shared" si="2"/>
+        <v>4C</v>
+      </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="str">
@@ -2010,7 +2190,7 @@
         <v>77</v>
       </c>
       <c r="C47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>M</v>
       </c>
       <c r="D47" t="s">
@@ -2028,6 +2208,10 @@
       <c r="H47" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="I47" t="str">
+        <f t="shared" si="2"/>
+        <v>4D</v>
+      </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" t="str">
@@ -2038,7 +2222,7 @@
         <v>78</v>
       </c>
       <c r="C48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>N</v>
       </c>
       <c r="D48" t="s">
@@ -2056,8 +2240,12 @@
       <c r="H48" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I48" t="str">
+        <f t="shared" si="2"/>
+        <v>4E</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>43B64C</v>
@@ -2066,7 +2254,7 @@
         <v>79</v>
       </c>
       <c r="C49" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>O</v>
       </c>
       <c r="D49" t="s">
@@ -2084,8 +2272,12 @@
       <c r="H49" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I49" t="str">
+        <f t="shared" si="2"/>
+        <v>4F</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>43B650</v>
@@ -2094,7 +2286,7 @@
         <v>80</v>
       </c>
       <c r="C50" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>P</v>
       </c>
       <c r="D50" t="s">
@@ -2112,8 +2304,12 @@
       <c r="H50" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I50" t="str">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>43B654</v>
@@ -2122,7 +2318,7 @@
         <v>81</v>
       </c>
       <c r="C51" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Q</v>
       </c>
       <c r="D51" t="s">
@@ -2140,8 +2336,12 @@
       <c r="H51" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I51" t="str">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>43B658</v>
@@ -2150,7 +2350,7 @@
         <v>82</v>
       </c>
       <c r="C52" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>R</v>
       </c>
       <c r="D52" t="s">
@@ -2168,8 +2368,12 @@
       <c r="H52" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I52" t="str">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="str">
         <f>DEC2HEX((B53 - 32)*4+HEX2DEC($M$1))</f>
         <v>43B65C</v>
@@ -2178,7 +2382,7 @@
         <v>83</v>
       </c>
       <c r="C53" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
       <c r="D53" t="s">
@@ -2196,8 +2400,12 @@
       <c r="H53" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I53" t="str">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>43B660</v>
@@ -2206,7 +2414,7 @@
         <v>84</v>
       </c>
       <c r="C54" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>T</v>
       </c>
       <c r="D54" t="s">
@@ -2224,8 +2432,12 @@
       <c r="H54" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I54" t="str">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>43B664</v>
@@ -2234,7 +2446,7 @@
         <v>85</v>
       </c>
       <c r="C55" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>U</v>
       </c>
       <c r="D55" t="s">
@@ -2252,8 +2464,12 @@
       <c r="H55" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I55" t="str">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="str">
         <f t="shared" si="0"/>
         <v>43B668</v>
@@ -2262,7 +2478,7 @@
         <v>86</v>
       </c>
       <c r="C56" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>V</v>
       </c>
       <c r="D56" t="s">
@@ -2280,8 +2496,12 @@
       <c r="H56" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I56" t="str">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="str">
         <f t="shared" si="0"/>
         <v>43B66C</v>
@@ -2290,7 +2510,7 @@
         <v>87</v>
       </c>
       <c r="C57" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>W</v>
       </c>
       <c r="D57" t="s">
@@ -2308,8 +2528,12 @@
       <c r="H57" s="4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I57" t="str">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="str">
         <f t="shared" si="0"/>
         <v>43B670</v>
@@ -2318,7 +2542,7 @@
         <v>88</v>
       </c>
       <c r="C58" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>X</v>
       </c>
       <c r="D58" t="s">
@@ -2336,8 +2560,12 @@
       <c r="H58" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I58" t="str">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="str">
         <f t="shared" si="0"/>
         <v>43B674</v>
@@ -2346,7 +2574,7 @@
         <v>89</v>
       </c>
       <c r="C59" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Y</v>
       </c>
       <c r="D59" t="s">
@@ -2364,8 +2592,12 @@
       <c r="H59" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I59" t="str">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="str">
         <f t="shared" si="0"/>
         <v>43B678</v>
@@ -2374,7 +2606,7 @@
         <v>90</v>
       </c>
       <c r="C60" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Z</v>
       </c>
       <c r="D60" t="s">
@@ -2392,8 +2624,12 @@
       <c r="H60" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I60" t="str">
+        <f t="shared" si="2"/>
+        <v>5A</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="str">
         <f t="shared" si="0"/>
         <v>43B67C</v>
@@ -2402,7 +2638,7 @@
         <v>91</v>
       </c>
       <c r="C61" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>[</v>
       </c>
       <c r="E61" s="4" t="s">
@@ -2417,8 +2653,12 @@
       <c r="H61" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I61" t="str">
+        <f t="shared" si="2"/>
+        <v>5B</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="str">
         <f t="shared" si="0"/>
         <v>43B680</v>
@@ -2427,7 +2667,7 @@
         <v>92</v>
       </c>
       <c r="C62" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>\</v>
       </c>
       <c r="E62" s="4" t="s">
@@ -2442,8 +2682,12 @@
       <c r="H62" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I62" t="str">
+        <f t="shared" si="2"/>
+        <v>5C</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="str">
         <f t="shared" si="0"/>
         <v>43B684</v>
@@ -2452,7 +2696,7 @@
         <v>93</v>
       </c>
       <c r="C63" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>]</v>
       </c>
       <c r="E63" s="4" t="s">
@@ -2467,8 +2711,12 @@
       <c r="H63" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I63" t="str">
+        <f t="shared" si="2"/>
+        <v>5D</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="str">
         <f t="shared" si="0"/>
         <v>43B688</v>
@@ -2477,7 +2725,7 @@
         <v>94</v>
       </c>
       <c r="C64" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>^</v>
       </c>
       <c r="E64" s="4" t="s">
@@ -2492,6 +2740,10 @@
       <c r="H64" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I64" t="str">
+        <f t="shared" si="2"/>
+        <v>5E</v>
+      </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" t="str">
@@ -2502,7 +2754,7 @@
         <v>95</v>
       </c>
       <c r="C65" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>_</v>
       </c>
       <c r="E65" s="4" t="s">
@@ -2517,17 +2769,21 @@
       <c r="H65" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I65" t="str">
+        <f t="shared" si="2"/>
+        <v>5F</v>
+      </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" t="str">
-        <f t="shared" ref="A66:A104" si="6">DEC2HEX((B66 - 32)*4+HEX2DEC($M$1))</f>
+        <f t="shared" ref="A66:A104" si="7">DEC2HEX((B66 - 32)*4+HEX2DEC($M$1))</f>
         <v>43B690</v>
       </c>
       <c r="B66">
         <v>96</v>
       </c>
       <c r="C66" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>`</v>
       </c>
       <c r="E66" s="4" t="s">
@@ -2542,17 +2798,21 @@
       <c r="H66" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I66" t="str">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B694</v>
       </c>
       <c r="B67">
         <v>97</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>a</v>
       </c>
       <c r="D67" t="s">
@@ -2570,17 +2830,21 @@
       <c r="H67" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="I67" t="str">
+        <f t="shared" ref="I67:I95" si="8">DEC2HEX(B67)</f>
+        <v>61</v>
+      </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B698</v>
       </c>
       <c r="B68">
         <v>98</v>
       </c>
       <c r="C68" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>b</v>
       </c>
       <c r="D68" t="s">
@@ -2597,6 +2861,10 @@
       </c>
       <c r="H68" s="4" t="s">
         <v>70</v>
+      </c>
+      <c r="I68" t="str">
+        <f t="shared" si="8"/>
+        <v>62</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.35">
@@ -2608,7 +2876,7 @@
         <v>99</v>
       </c>
       <c r="C69" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>c</v>
       </c>
       <c r="D69" t="s">
@@ -2626,17 +2894,21 @@
       <c r="H69" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="I69" t="str">
+        <f t="shared" si="8"/>
+        <v>63</v>
+      </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6A0</v>
       </c>
       <c r="B70">
         <v>100</v>
       </c>
       <c r="C70" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>d</v>
       </c>
       <c r="D70" t="s">
@@ -2654,17 +2926,21 @@
       <c r="H70" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="I70" t="str">
+        <f t="shared" si="8"/>
+        <v>64</v>
+      </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6A4</v>
       </c>
       <c r="B71">
         <v>101</v>
       </c>
       <c r="C71" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>e</v>
       </c>
       <c r="D71" t="s">
@@ -2682,17 +2958,21 @@
       <c r="H71" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="I71" t="str">
+        <f t="shared" si="8"/>
+        <v>65</v>
+      </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6A8</v>
       </c>
       <c r="B72">
         <v>102</v>
       </c>
       <c r="C72" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>f</v>
       </c>
       <c r="D72" t="s">
@@ -2710,18 +2990,22 @@
       <c r="H72" s="4" t="s">
         <v>72</v>
       </c>
+      <c r="I72" t="str">
+        <f t="shared" si="8"/>
+        <v>66</v>
+      </c>
       <c r="J72" s="4"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6AC</v>
       </c>
       <c r="B73">
         <v>103</v>
       </c>
       <c r="C73" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>g</v>
       </c>
       <c r="D73" t="s">
@@ -2739,17 +3023,21 @@
       <c r="H73" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="I73" t="str">
+        <f t="shared" si="8"/>
+        <v>67</v>
+      </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6B0</v>
       </c>
       <c r="B74">
         <v>104</v>
       </c>
       <c r="C74" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>h</v>
       </c>
       <c r="D74" t="s">
@@ -2767,17 +3055,21 @@
       <c r="H74" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="I74" t="str">
+        <f t="shared" si="8"/>
+        <v>68</v>
+      </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6B4</v>
       </c>
       <c r="B75">
         <v>105</v>
       </c>
       <c r="C75" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>i</v>
       </c>
       <c r="D75" t="s">
@@ -2795,17 +3087,21 @@
       <c r="H75" s="4" t="s">
         <v>73</v>
       </c>
+      <c r="I75" t="str">
+        <f t="shared" si="8"/>
+        <v>69</v>
+      </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6B8</v>
       </c>
       <c r="B76">
         <v>106</v>
       </c>
       <c r="C76" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>j</v>
       </c>
       <c r="D76" t="s">
@@ -2823,17 +3119,21 @@
       <c r="H76" s="4" t="s">
         <v>72</v>
       </c>
+      <c r="I76" t="str">
+        <f t="shared" si="8"/>
+        <v>6A</v>
+      </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6BC</v>
       </c>
       <c r="B77">
         <v>107</v>
       </c>
       <c r="C77" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>k</v>
       </c>
       <c r="D77" t="s">
@@ -2851,18 +3151,22 @@
       <c r="H77" s="4" t="s">
         <v>72</v>
       </c>
+      <c r="I77" t="str">
+        <f t="shared" si="8"/>
+        <v>6B</v>
+      </c>
       <c r="L77" s="2"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6C0</v>
       </c>
       <c r="B78">
         <v>108</v>
       </c>
       <c r="C78" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>l</v>
       </c>
       <c r="D78" t="s">
@@ -2880,17 +3184,21 @@
       <c r="H78" s="4" t="s">
         <v>73</v>
       </c>
+      <c r="I78" t="str">
+        <f t="shared" si="8"/>
+        <v>6C</v>
+      </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6C4</v>
       </c>
       <c r="B79">
         <v>109</v>
       </c>
       <c r="C79" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>m</v>
       </c>
       <c r="D79" t="s">
@@ -2908,17 +3216,21 @@
       <c r="H79" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="I79" t="str">
+        <f t="shared" si="8"/>
+        <v>6D</v>
+      </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6C8</v>
       </c>
       <c r="B80">
         <v>110</v>
       </c>
       <c r="C80" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>n</v>
       </c>
       <c r="D80" t="s">
@@ -2936,17 +3248,21 @@
       <c r="H80" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I80" t="str">
+        <f t="shared" si="8"/>
+        <v>6E</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6CC</v>
       </c>
       <c r="B81">
         <v>111</v>
       </c>
       <c r="C81" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>o</v>
       </c>
       <c r="D81" t="s">
@@ -2964,17 +3280,21 @@
       <c r="H81" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I81" t="str">
+        <f t="shared" si="8"/>
+        <v>6F</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6D0</v>
       </c>
       <c r="B82">
         <v>112</v>
       </c>
       <c r="C82" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>p</v>
       </c>
       <c r="D82" t="s">
@@ -2992,17 +3312,21 @@
       <c r="H82" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I82" t="str">
+        <f t="shared" si="8"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6D4</v>
       </c>
       <c r="B83">
         <v>113</v>
       </c>
       <c r="C83" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>q</v>
       </c>
       <c r="D83" t="s">
@@ -3020,17 +3344,21 @@
       <c r="H83" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I83" t="str">
+        <f t="shared" si="8"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6D8</v>
       </c>
       <c r="B84">
         <v>114</v>
       </c>
       <c r="C84" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>r</v>
       </c>
       <c r="D84" t="s">
@@ -3048,17 +3376,21 @@
       <c r="H84" s="4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I84" t="str">
+        <f t="shared" si="8"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6DC</v>
       </c>
       <c r="B85">
         <v>115</v>
       </c>
       <c r="C85" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>s</v>
       </c>
       <c r="D85" t="s">
@@ -3076,17 +3408,21 @@
       <c r="H85" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I85" t="str">
+        <f t="shared" si="8"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6E0</v>
       </c>
       <c r="B86">
         <v>116</v>
       </c>
       <c r="C86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>t</v>
       </c>
       <c r="D86" t="s">
@@ -3104,17 +3440,21 @@
       <c r="H86" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I86" t="str">
+        <f t="shared" si="8"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6E4</v>
       </c>
       <c r="B87">
         <v>117</v>
       </c>
       <c r="C87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>u</v>
       </c>
       <c r="D87" t="s">
@@ -3132,17 +3472,21 @@
       <c r="H87" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I87" t="str">
+        <f t="shared" si="8"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6E8</v>
       </c>
       <c r="B88">
         <v>118</v>
       </c>
       <c r="C88" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>v</v>
       </c>
       <c r="D88" t="s">
@@ -3160,17 +3504,21 @@
       <c r="H88" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I88" t="str">
+        <f t="shared" si="8"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6EC</v>
       </c>
       <c r="B89">
         <v>119</v>
       </c>
       <c r="C89" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>w</v>
       </c>
       <c r="D89" t="s">
@@ -3188,17 +3536,21 @@
       <c r="H89" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I89" t="str">
+        <f t="shared" si="8"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6F0</v>
       </c>
       <c r="B90">
         <v>120</v>
       </c>
       <c r="C90" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>x</v>
       </c>
       <c r="D90" t="s">
@@ -3216,17 +3568,21 @@
       <c r="H90" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I90" t="str">
+        <f t="shared" si="8"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6F4</v>
       </c>
       <c r="B91">
         <v>121</v>
       </c>
       <c r="C91" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>y</v>
       </c>
       <c r="D91" t="s">
@@ -3244,17 +3600,21 @@
       <c r="H91" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I91" t="str">
+        <f t="shared" si="8"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6F8</v>
       </c>
       <c r="B92">
         <v>122</v>
       </c>
       <c r="C92" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>z</v>
       </c>
       <c r="D92" t="s">
@@ -3272,17 +3632,21 @@
       <c r="H92" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I92" t="str">
+        <f t="shared" si="8"/>
+        <v>7A</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B6FC</v>
       </c>
       <c r="B93">
         <v>123</v>
       </c>
       <c r="C93" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>{</v>
       </c>
       <c r="E93" s="4" t="s">
@@ -3297,17 +3661,21 @@
       <c r="H93" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I93" t="str">
+        <f t="shared" si="8"/>
+        <v>7B</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B700</v>
       </c>
       <c r="B94">
         <v>124</v>
       </c>
       <c r="C94" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>|</v>
       </c>
       <c r="E94" s="4" t="s">
@@ -3322,17 +3690,21 @@
       <c r="H94" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I94" t="str">
+        <f t="shared" si="8"/>
+        <v>7C</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B704</v>
       </c>
       <c r="B95">
         <v>125</v>
       </c>
       <c r="C95" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>}</v>
       </c>
       <c r="E95" s="4" t="s">
@@ -3347,17 +3719,21 @@
       <c r="H95" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I95" t="str">
+        <f t="shared" si="8"/>
+        <v>7D</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B708</v>
       </c>
       <c r="B96">
         <v>126</v>
       </c>
       <c r="C96" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>~</v>
       </c>
       <c r="E96" s="4" t="s">
@@ -3375,7 +3751,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B70C</v>
       </c>
       <c r="B97">
@@ -3399,14 +3775,14 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B710</v>
       </c>
       <c r="B98">
         <v>128</v>
       </c>
       <c r="C98" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>€</v>
       </c>
       <c r="E98" s="4" t="s">
@@ -3424,14 +3800,14 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B714</v>
       </c>
       <c r="B99">
         <v>129</v>
       </c>
       <c r="C99" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v></v>
       </c>
       <c r="E99" s="4" t="s">
@@ -3449,14 +3825,14 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B718</v>
       </c>
       <c r="B100">
         <v>130</v>
       </c>
       <c r="C100" t="str">
-        <f t="shared" ref="C100:C109" si="7">CHAR(B100)</f>
+        <f t="shared" ref="C100:C109" si="9">CHAR(B100)</f>
         <v>‚</v>
       </c>
       <c r="E100" s="4" t="s">
@@ -3474,14 +3850,14 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B71C</v>
       </c>
       <c r="B101">
         <v>131</v>
       </c>
       <c r="C101" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>ƒ</v>
       </c>
       <c r="E101" s="4" t="s">
@@ -3499,14 +3875,14 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B720</v>
       </c>
       <c r="B102">
         <v>132</v>
       </c>
       <c r="C102" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>„</v>
       </c>
       <c r="E102" s="4" t="s">
@@ -3524,14 +3900,14 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B724</v>
       </c>
       <c r="B103">
         <v>133</v>
       </c>
       <c r="C103" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>…</v>
       </c>
       <c r="E103" s="4" t="s">
@@ -3549,14 +3925,14 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43B728</v>
       </c>
       <c r="B104">
         <v>134</v>
       </c>
       <c r="C104" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>†</v>
       </c>
       <c r="E104" s="4" t="s">
@@ -3577,7 +3953,7 @@
         <v>135</v>
       </c>
       <c r="C105" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>‡</v>
       </c>
       <c r="E105" s="4" t="s">
@@ -3598,7 +3974,7 @@
         <v>136</v>
       </c>
       <c r="C106" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>ˆ</v>
       </c>
       <c r="E106" s="4" t="s">
@@ -3619,7 +3995,7 @@
         <v>137</v>
       </c>
       <c r="C107" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>‰</v>
       </c>
       <c r="E107" s="4" t="s">
@@ -3640,7 +4016,7 @@
         <v>138</v>
       </c>
       <c r="C108" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>Š</v>
       </c>
       <c r="E108" s="4" t="s">
@@ -3661,7 +4037,7 @@
         <v>139</v>
       </c>
       <c r="C109" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>‹</v>
       </c>
       <c r="E109" s="4" t="s">

</xml_diff>

<commit_message>
Fix characters width issues based on sreenshots
Adjust font
</commit_message>
<xml_diff>
--- a/2_translated/font/VWF_Properties.xlsx
+++ b/2_translated/font/VWF_Properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forti\Documents\GitHub\Super-Robot-Wars-Z\2_translated\font\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428C279F-97AD-4F32-A662-05AF901C227B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326A0D50-CE0E-44DC-BFB2-2D27073F4AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{4CE9F589-6C49-444B-92C3-C90A26708452}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="88">
   <si>
     <t>Ａ</t>
   </si>
@@ -284,19 +284,22 @@
     <t>06</t>
   </si>
   <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Width_00</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>≥</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
     <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>Width_00</t>
-  </si>
-  <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t>≥</t>
   </si>
 </sst>
 </file>
@@ -684,8 +687,8 @@
   <dimension ref="A1:M114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -718,7 +721,7 @@
         <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>74</v>
@@ -968,13 +971,13 @@
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G9" t="s">
-        <v>57</v>
+        <v>78</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>68</v>
@@ -1128,13 +1131,13 @@
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" t="s">
-        <v>65</v>
-      </c>
-      <c r="G14" t="s">
-        <v>57</v>
+        <v>84</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>68</v>
@@ -1192,13 +1195,13 @@
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" t="s">
-        <v>65</v>
-      </c>
-      <c r="G16" t="s">
-        <v>57</v>
+        <v>84</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>68</v>
@@ -1223,8 +1226,8 @@
         <v>/</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="4" t="s">
-        <v>64</v>
+      <c r="E17" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="F17" t="s">
         <v>65</v>
@@ -1802,13 +1805,13 @@
         <v>0</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F35" t="s">
         <v>64</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>67</v>
@@ -1875,8 +1878,8 @@
       <c r="F37" t="s">
         <v>64</v>
       </c>
-      <c r="G37" t="s">
-        <v>57</v>
+      <c r="G37" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>69</v>
@@ -1938,7 +1941,7 @@
         <v>4</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>62</v>
@@ -1970,13 +1973,13 @@
         <v>5</v>
       </c>
       <c r="E40" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G40" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="F40" t="s">
-        <v>80</v>
-      </c>
-      <c r="G40" t="s">
-        <v>57</v>
       </c>
       <c r="H40" s="4" t="s">
         <v>70</v>
@@ -2069,10 +2072,10 @@
         <v>78</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G43" t="s">
-        <v>57</v>
+        <v>84</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>57</v>
@@ -2097,14 +2100,14 @@
       <c r="D44" t="s">
         <v>9</v>
       </c>
-      <c r="E44" s="4">
-        <v>11</v>
-      </c>
-      <c r="F44" t="s">
-        <v>83</v>
-      </c>
-      <c r="G44" t="s">
-        <v>57</v>
+      <c r="E44" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>70</v>
@@ -2162,7 +2165,7 @@
         <v>11</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>62</v>
@@ -2200,7 +2203,7 @@
         <v>63</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>67</v>
@@ -2264,7 +2267,7 @@
         <v>65</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>65</v>
@@ -2354,13 +2357,13 @@
         <v>17</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G52" t="s">
-        <v>57</v>
+      <c r="G52" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>68</v>
@@ -2418,7 +2421,7 @@
         <v>19</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F54" t="s">
         <v>65</v>
@@ -2450,13 +2453,13 @@
         <v>20</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="F55" t="s">
         <v>62</v>
       </c>
-      <c r="G55" t="s">
-        <v>57</v>
+      <c r="G55" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>69</v>
@@ -2514,13 +2517,13 @@
         <v>22</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G57" t="s">
-        <v>57</v>
+      <c r="G57" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="H57" s="4" t="s">
         <v>71</v>
@@ -2610,13 +2613,13 @@
         <v>25</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G60" t="s">
-        <v>57</v>
+        <v>80</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="H60" s="4" t="s">
         <v>68</v>
@@ -3076,10 +3079,10 @@
         <v>78</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H75" s="4" t="s">
         <v>73</v>
@@ -3170,10 +3173,10 @@
         <v>37</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>75</v>
@@ -3208,7 +3211,7 @@
         <v>63</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H79" s="4" t="s">
         <v>67</v>
@@ -3233,8 +3236,8 @@
       <c r="D80" t="s">
         <v>39</v>
       </c>
-      <c r="E80" s="4" t="s">
-        <v>77</v>
+      <c r="E80" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>79</v>
@@ -3271,8 +3274,8 @@
       <c r="F81" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G81" t="s">
-        <v>57</v>
+      <c r="G81" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="H81" s="4" t="s">
         <v>70</v>
@@ -3362,7 +3365,7 @@
         <v>43</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>81</v>
@@ -3586,7 +3589,7 @@
         <v>50</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F91" t="s">
         <v>80</v>
@@ -3755,7 +3758,7 @@
         <v>127</v>
       </c>
       <c r="C97" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E97" s="4" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
Update font and change status to proofread
Update Yes/no Position
</commit_message>
<xml_diff>
--- a/2_translated/font/VWF_Properties.xlsx
+++ b/2_translated/font/VWF_Properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forti\Documents\GitHub\Super-Robot-Wars-Z\2_translated\font\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B2AAAD-CF6F-4319-95C7-0D1D834FC509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EACA638-B922-44E2-BF3B-211EEC4A3FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{4CE9F589-6C49-444B-92C3-C90A26708452}"/>
+    <workbookView xWindow="0" yWindow="100" windowWidth="19200" windowHeight="11180" xr2:uid="{4CE9F589-6C49-444B-92C3-C90A26708452}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -687,21 +687,21 @@
   <dimension ref="A1:M114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G72" sqref="G72"/>
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I88" sqref="I88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" customWidth="1"/>
+    <col min="8" max="8" width="14.26953125" customWidth="1"/>
+    <col min="11" max="11" width="5.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
@@ -733,7 +733,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
         <f t="shared" ref="A2:A65" si="0">DEC2HEX((B2 - 32)*4+HEX2DEC($M$1))</f>
         <v>43B590</v>
@@ -765,7 +765,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>43B594</v>
@@ -797,7 +797,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>43B598</v>
@@ -829,7 +829,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>43B59C</v>
@@ -861,7 +861,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>43B5A0</v>
@@ -893,7 +893,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>43B5A4</v>
@@ -925,7 +925,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>43B5A8</v>
@@ -957,7 +957,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>43B5AC</v>
@@ -989,7 +989,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>43B5B0</v>
@@ -1021,7 +1021,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>43B5B4</v>
@@ -1053,7 +1053,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>43B5B8</v>
@@ -1085,7 +1085,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>43B5BC</v>
@@ -1117,7 +1117,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>43B5C0</v>
@@ -1149,7 +1149,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>43B5C4</v>
@@ -1181,7 +1181,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>43B5C8</v>
@@ -1213,7 +1213,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>43B5CC</v>
@@ -1245,7 +1245,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>43B5D0</v>
@@ -1277,7 +1277,7 @@
       <c r="L18" s="1"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>43B5D4</v>
@@ -1309,7 +1309,7 @@
       <c r="L19" s="1"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>43B5D8</v>
@@ -1341,7 +1341,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>43B5DC</v>
@@ -1373,7 +1373,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>43B5E0</v>
@@ -1405,7 +1405,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>43B5E4</v>
@@ -1437,7 +1437,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>43B5E8</v>
@@ -1469,7 +1469,7 @@
       <c r="L24" s="1"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>43B5EC</v>
@@ -1501,7 +1501,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>43B5F0</v>
@@ -1533,7 +1533,7 @@
       <c r="L26" s="1"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>43B5F4</v>
@@ -1565,7 +1565,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>43B5F8</v>
@@ -1597,7 +1597,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>43B5FC</v>
@@ -1629,7 +1629,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="2"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>43B600</v>
@@ -1661,7 +1661,7 @@
       <c r="L30" s="1"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>43B604</v>
@@ -1693,7 +1693,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>43B608</v>
@@ -1725,7 +1725,7 @@
       <c r="L32" s="1"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>43B60C</v>
@@ -1757,7 +1757,7 @@
       <c r="L33" s="1"/>
       <c r="M33" s="2"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>43B610</v>
@@ -1789,7 +1789,7 @@
       <c r="L34" s="1"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>43B614</v>
@@ -1825,7 +1825,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>43B618</v>
@@ -1857,7 +1857,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>43B61C</v>
@@ -1893,7 +1893,7 @@
         <v>43B65C</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>43B620</v>
@@ -1914,8 +1914,8 @@
       <c r="F38" t="s">
         <v>65</v>
       </c>
-      <c r="G38" t="s">
-        <v>57</v>
+      <c r="G38" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="H38" s="4" t="s">
         <v>68</v>
@@ -1925,7 +1925,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>43B624</v>
@@ -1957,7 +1957,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>43B628</v>
@@ -1989,7 +1989,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" t="str">
         <f>DEC2HEX((B41 - 32)*4+HEX2DEC($M$1))</f>
         <v>43B62C</v>
@@ -2021,7 +2021,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>43B630</v>
@@ -2053,7 +2053,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>43B634</v>
@@ -2085,7 +2085,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>43B638</v>
@@ -2117,7 +2117,7 @@
         <v>4A</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>43B63C</v>
@@ -2149,7 +2149,7 @@
         <v>4B</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>43B640</v>
@@ -2181,7 +2181,7 @@
         <v>4C</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>43B644</v>
@@ -2213,7 +2213,7 @@
         <v>4D</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>43B648</v>
@@ -2245,7 +2245,7 @@
         <v>4E</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>43B64C</v>
@@ -2277,7 +2277,7 @@
         <v>4F</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>43B650</v>
@@ -2309,7 +2309,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>43B654</v>
@@ -2341,7 +2341,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>43B658</v>
@@ -2373,7 +2373,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="str">
         <f>DEC2HEX((B53 - 32)*4+HEX2DEC($M$1))</f>
         <v>43B65C</v>
@@ -2405,7 +2405,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>43B660</v>
@@ -2437,7 +2437,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>43B664</v>
@@ -2469,7 +2469,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="str">
         <f t="shared" si="0"/>
         <v>43B668</v>
@@ -2501,7 +2501,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="str">
         <f t="shared" si="0"/>
         <v>43B66C</v>
@@ -2533,7 +2533,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="str">
         <f t="shared" si="0"/>
         <v>43B670</v>
@@ -2565,7 +2565,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="str">
         <f t="shared" si="0"/>
         <v>43B674</v>
@@ -2597,7 +2597,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="str">
         <f t="shared" si="0"/>
         <v>43B678</v>
@@ -2629,7 +2629,7 @@
         <v>5A</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="str">
         <f t="shared" si="0"/>
         <v>43B67C</v>
@@ -2658,7 +2658,7 @@
         <v>5B</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="str">
         <f t="shared" si="0"/>
         <v>43B680</v>
@@ -2687,7 +2687,7 @@
         <v>5C</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="str">
         <f t="shared" si="0"/>
         <v>43B684</v>
@@ -2716,7 +2716,7 @@
         <v>5D</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="str">
         <f t="shared" si="0"/>
         <v>43B688</v>
@@ -2745,7 +2745,7 @@
         <v>5E</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" t="str">
         <f t="shared" si="0"/>
         <v>43B68C</v>
@@ -2774,7 +2774,7 @@
         <v>5F</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" t="str">
         <f t="shared" ref="A66:A104" si="7">DEC2HEX((B66 - 32)*4+HEX2DEC($M$1))</f>
         <v>43B690</v>
@@ -2803,7 +2803,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" t="str">
         <f t="shared" si="7"/>
         <v>43B694</v>
@@ -2835,7 +2835,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" t="str">
         <f t="shared" si="7"/>
         <v>43B698</v>
@@ -2867,7 +2867,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" t="str">
         <f>DEC2HEX((B69 - 32)*4+HEX2DEC($M$1))</f>
         <v>43B69C</v>
@@ -2899,7 +2899,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" t="str">
         <f t="shared" si="7"/>
         <v>43B6A0</v>
@@ -2931,7 +2931,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" t="str">
         <f t="shared" si="7"/>
         <v>43B6A4</v>
@@ -2963,7 +2963,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" t="str">
         <f t="shared" si="7"/>
         <v>43B6A8</v>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="J72" s="4"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" t="str">
         <f t="shared" si="7"/>
         <v>43B6AC</v>
@@ -3028,7 +3028,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" t="str">
         <f t="shared" si="7"/>
         <v>43B6B0</v>
@@ -3060,7 +3060,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" t="str">
         <f t="shared" si="7"/>
         <v>43B6B4</v>
@@ -3092,7 +3092,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" t="str">
         <f t="shared" si="7"/>
         <v>43B6B8</v>
@@ -3124,7 +3124,7 @@
         <v>6A</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" t="str">
         <f t="shared" si="7"/>
         <v>43B6BC</v>
@@ -3157,7 +3157,7 @@
       </c>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" t="str">
         <f t="shared" si="7"/>
         <v>43B6C0</v>
@@ -3189,7 +3189,7 @@
         <v>6C</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" t="str">
         <f t="shared" si="7"/>
         <v>43B6C4</v>
@@ -3221,7 +3221,7 @@
         <v>6D</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" t="str">
         <f t="shared" si="7"/>
         <v>43B6C8</v>
@@ -3253,7 +3253,7 @@
         <v>6E</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="str">
         <f t="shared" si="7"/>
         <v>43B6CC</v>
@@ -3285,7 +3285,7 @@
         <v>6F</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="str">
         <f t="shared" si="7"/>
         <v>43B6D0</v>
@@ -3317,7 +3317,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="str">
         <f t="shared" si="7"/>
         <v>43B6D4</v>
@@ -3349,7 +3349,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="str">
         <f t="shared" si="7"/>
         <v>43B6D8</v>
@@ -3381,7 +3381,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="str">
         <f t="shared" si="7"/>
         <v>43B6DC</v>
@@ -3413,7 +3413,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="str">
         <f t="shared" si="7"/>
         <v>43B6E0</v>
@@ -3445,7 +3445,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="str">
         <f t="shared" si="7"/>
         <v>43B6E4</v>
@@ -3466,8 +3466,8 @@
       <c r="F87" t="s">
         <v>80</v>
       </c>
-      <c r="G87" t="s">
-        <v>57</v>
+      <c r="G87" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="H87" s="4" t="s">
         <v>70</v>
@@ -3477,7 +3477,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="str">
         <f t="shared" si="7"/>
         <v>43B6E8</v>
@@ -3509,7 +3509,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="str">
         <f t="shared" si="7"/>
         <v>43B6EC</v>
@@ -3541,7 +3541,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="str">
         <f t="shared" si="7"/>
         <v>43B6F0</v>
@@ -3573,7 +3573,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="str">
         <f t="shared" si="7"/>
         <v>43B6F4</v>
@@ -3605,7 +3605,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="str">
         <f t="shared" si="7"/>
         <v>43B6F8</v>
@@ -3637,7 +3637,7 @@
         <v>7A</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="str">
         <f t="shared" si="7"/>
         <v>43B6FC</v>
@@ -3666,7 +3666,7 @@
         <v>7B</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="str">
         <f t="shared" si="7"/>
         <v>43B700</v>
@@ -3695,7 +3695,7 @@
         <v>7C</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="str">
         <f t="shared" si="7"/>
         <v>43B704</v>
@@ -3724,7 +3724,7 @@
         <v>7D</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="str">
         <f t="shared" si="7"/>
         <v>43B708</v>
@@ -3749,7 +3749,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" t="str">
         <f t="shared" si="7"/>
         <v>43B70C</v>
@@ -3773,7 +3773,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" t="str">
         <f t="shared" si="7"/>
         <v>43B710</v>
@@ -3798,7 +3798,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" t="str">
         <f t="shared" si="7"/>
         <v>43B714</v>
@@ -3823,7 +3823,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" t="str">
         <f t="shared" si="7"/>
         <v>43B718</v>
@@ -3848,7 +3848,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" t="str">
         <f t="shared" si="7"/>
         <v>43B71C</v>
@@ -3873,7 +3873,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" t="str">
         <f t="shared" si="7"/>
         <v>43B720</v>
@@ -3898,7 +3898,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" t="str">
         <f t="shared" si="7"/>
         <v>43B724</v>
@@ -3923,7 +3923,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" t="str">
         <f t="shared" si="7"/>
         <v>43B728</v>
@@ -3948,7 +3948,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B105">
         <v>135</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B106">
         <v>136</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B107">
         <v>137</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B108">
         <v>138</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B109">
         <v>139</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="114" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K114" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Add 3 missing translations
</commit_message>
<xml_diff>
--- a/2_translated/font/VWF_Properties.xlsx
+++ b/2_translated/font/VWF_Properties.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forti\Documents\GitHub\Super-Robot-Wars-Z\2_translated\font\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326A0D50-CE0E-44DC-BFB2-2D27073F4AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F995FD-4CA6-4215-81CB-21341A3C9402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{4CE9F589-6C49-444B-92C3-C90A26708452}"/>
   </bookViews>
@@ -687,8 +687,8 @@
   <dimension ref="A1:M114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3736,11 +3736,11 @@
         <f t="shared" si="6"/>
         <v>~</v>
       </c>
-      <c r="E96" s="4" t="s">
-        <v>76</v>
+      <c r="E96" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="F96" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="G96" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
Hacking - Pilot and Mech Info (#105)
* First hacking pass

* Hack

Hacking

* Translate missing entries
</commit_message>
<xml_diff>
--- a/2_translated/font/VWF_Properties.xlsx
+++ b/2_translated/font/VWF_Properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forti\Documents\GitHub\Super-Robot-Wars-Z\2_translated\font\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EACA638-B922-44E2-BF3B-211EEC4A3FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A9B224-3AAB-4AEC-BC8D-6F86CF4362D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="100" windowWidth="19200" windowHeight="11180" xr2:uid="{4CE9F589-6C49-444B-92C3-C90A26708452}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{4CE9F589-6C49-444B-92C3-C90A26708452}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -687,8 +687,8 @@
   <dimension ref="A1:M114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I88" sqref="I88"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1229,8 +1229,8 @@
       <c r="E17" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F17" t="s">
-        <v>65</v>
+      <c r="F17" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="G17" t="s">
         <v>57</v>

</xml_diff>